<commit_message>
Added ToughGFX project completed Splash and Main Screen
</commit_message>
<xml_diff>
--- a/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
+++ b/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EE55399-EB52-4406-8FBF-98EB8EC9EF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CE3771F-D937-41C1-8578-0BB4E0DE6C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -127,10 +127,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>2/25/2025</t>
-  </si>
-  <si>
-    <t>5:13:38 AM</t>
+    <t>2/28/2025</t>
+  </si>
+  <si>
+    <t>10:23:31 AM</t>
   </si>
   <si>
     <t>Arbitrary Power Booster</t>
@@ -1243,7 +1243,7 @@
     <t>245</t>
   </si>
   <si>
-    <t>2/25/2025 5:13:38 AM</t>
+    <t>2/28/2025 10:23:31 AM</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -2625,11 +2625,11 @@
       </c>
       <c r="E8" s="38">
         <f ca="1">TODAY()</f>
-        <v>45713</v>
+        <v>45716</v>
       </c>
       <c r="F8" s="39">
         <f ca="1">NOW()</f>
-        <v>45713.218288194446</v>
+        <v>45716.434250694445</v>
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>

</xml_diff>

<commit_message>
Added more to TouchGFX screens. Created Test Plan. Added notes to schematic
</commit_message>
<xml_diff>
--- a/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
+++ b/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CE3771F-D937-41C1-8578-0BB4E0DE6C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2CB02FE-BDA2-4B0E-BC24-354651F729BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -130,7 +130,7 @@
     <t>2/28/2025</t>
   </si>
   <si>
-    <t>10:23:31 AM</t>
+    <t>6:01:02 PM</t>
   </si>
   <si>
     <t>Arbitrary Power Booster</t>
@@ -1243,7 +1243,7 @@
     <t>245</t>
   </si>
   <si>
-    <t>2/28/2025 10:23:31 AM</t>
+    <t>2/28/2025 6:01:02 PM</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="F8" s="39">
         <f ca="1">NOW()</f>
-        <v>45716.434250694445</v>
+        <v>45716.751401620371</v>
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>

</xml_diff>

<commit_message>
Touch GFX way to increment set digits and refinement to variable names. Added LTSpice circuit to add back in Vbe offset of current booster.
</commit_message>
<xml_diff>
--- a/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
+++ b/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2CB02FE-BDA2-4B0E-BC24-354651F729BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{720C984A-A245-4F93-8882-AA3619980FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -127,10 +127,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>2/28/2025</t>
-  </si>
-  <si>
-    <t>6:01:02 PM</t>
+    <t>3/1/2025</t>
+  </si>
+  <si>
+    <t>7:32:12 AM</t>
   </si>
   <si>
     <t>Arbitrary Power Booster</t>
@@ -1243,7 +1243,7 @@
     <t>245</t>
   </si>
   <si>
-    <t>2/28/2025 6:01:02 PM</t>
+    <t>3/1/2025 7:32:12 AM</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -2625,11 +2625,11 @@
       </c>
       <c r="E8" s="38">
         <f ca="1">TODAY()</f>
-        <v>45716</v>
+        <v>45717</v>
       </c>
       <c r="F8" s="39">
         <f ca="1">NOW()</f>
-        <v>45716.751401620371</v>
+        <v>45717.314340740741</v>
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>

</xml_diff>

<commit_message>
Created a REV1 zip for PCB Build. Modified .ioc file and for MAIN_PWR_EN. Clean up and notes added to project
</commit_message>
<xml_diff>
--- a/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
+++ b/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{720C984A-A245-4F93-8882-AA3619980FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IMR_Projects\IMR\Arb_Power_Booster\Hardware\Arb_Power_Booster\Default Configuration\Outputs\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CA1B07-1127-435C-AC42-941F1DFF38EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -1823,7 +1828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1855,20 +1860,8 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1901,9 +1894,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1925,13 +1915,7 @@
     <xf numFmtId="164" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1947,10 +1931,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1985,6 +1965,51 @@
     <xf numFmtId="166" fontId="7" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1993,50 +2018,54 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="6" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2466,8 +2495,8 @@
   </sheetPr>
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2477,7 +2506,7 @@
     <col min="3" max="3" width="8.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="50.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="80" customWidth="1"/>
     <col min="7" max="10" width="25.7109375" style="1" customWidth="1"/>
     <col min="11" max="12" width="10.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" customWidth="1"/>
@@ -2485,2492 +2514,2492 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="F1" s="68"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="22"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="52" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="64" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28" t="s">
+      <c r="F3" s="70"/>
+      <c r="G3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="30"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="26"/>
     </row>
     <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="31" t="s">
+      <c r="F4" s="70"/>
+      <c r="G4" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="30"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="26"/>
     </row>
     <row r="5" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="32" t="s">
+      <c r="F5" s="70"/>
+      <c r="G5" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="30"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="26"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="36"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="29" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="63" t="s">
+      <c r="F7" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="30"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="34">
         <f ca="1">TODAY()</f>
-        <v>45717</v>
-      </c>
-      <c r="F8" s="39">
+        <v>45719</v>
+      </c>
+      <c r="F8" s="73">
         <f ca="1">NOW()</f>
-        <v>45717.314340740741</v>
-      </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="30"/>
+        <v>45719.318134953704</v>
+      </c>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="45" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="57" t="s">
         <v>218</v>
       </c>
-      <c r="H9" s="66" t="s">
+      <c r="H9" s="57" t="s">
         <v>242</v>
       </c>
-      <c r="I9" s="66" t="s">
+      <c r="I9" s="57" t="s">
         <v>302</v>
       </c>
-      <c r="J9" s="66" t="s">
+      <c r="J9" s="57" t="s">
         <v>305</v>
       </c>
-      <c r="K9" s="66" t="s">
+      <c r="K9" s="57" t="s">
         <v>364</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="L9" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="48">
-        <f>ROW(B10) - ROW($B$9)</f>
+      <c r="A10" s="12"/>
+      <c r="B10" s="41">
+        <f t="shared" ref="B10:B41" si="0">ROW(B10) - ROW($B$9)</f>
         <v>1</v>
       </c>
-      <c r="C10" s="50">
+      <c r="C10" s="43">
         <v>6</v>
       </c>
-      <c r="D10" s="67" t="s">
+      <c r="D10" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="67" t="s">
+      <c r="E10" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="69" t="s">
+      <c r="F10" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="G10" s="69" t="s">
+      <c r="G10" s="60" t="s">
         <v>219</v>
       </c>
-      <c r="H10" s="69" t="s">
+      <c r="H10" s="60" t="s">
         <v>243</v>
       </c>
-      <c r="I10" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J10" s="69" t="s">
+      <c r="I10" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J10" s="60" t="s">
         <v>306</v>
       </c>
-      <c r="K10" s="70" t="s">
+      <c r="K10" s="61" t="s">
         <v>365</v>
       </c>
-      <c r="L10" s="55">
+      <c r="L10" s="48">
         <f>C10*K10</f>
         <v>8.4599999999999991</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="49">
-        <f>ROW(B11) - ROW($B$9)</f>
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="42">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="44">
         <v>3</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="68" t="s">
+      <c r="E11" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="68" t="s">
+      <c r="F11" s="59" t="s">
         <v>160</v>
       </c>
-      <c r="G11" s="68" t="s">
+      <c r="G11" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="H11" s="68" t="s">
+      <c r="H11" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="I11" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J11" s="68" t="s">
+      <c r="I11" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J11" s="59" t="s">
         <v>307</v>
       </c>
-      <c r="K11" s="71" t="s">
+      <c r="K11" s="62" t="s">
         <v>366</v>
       </c>
-      <c r="L11" s="57">
-        <f t="shared" ref="L11:L68" si="0">C11*K11</f>
+      <c r="L11" s="50">
+        <f t="shared" ref="L11" si="1">C11*K11</f>
         <v>0.84000000000000008</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="48">
-        <f>ROW(B12) - ROW($B$9)</f>
+      <c r="A12" s="12"/>
+      <c r="B12" s="41">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C12" s="50">
+      <c r="C12" s="43">
         <v>26</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="69" t="s">
+      <c r="F12" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="G12" s="60" t="s">
         <v>221</v>
       </c>
-      <c r="H12" s="69" t="s">
+      <c r="H12" s="60" t="s">
         <v>245</v>
       </c>
-      <c r="I12" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J12" s="69" t="s">
+      <c r="I12" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J12" s="60" t="s">
         <v>308</v>
       </c>
-      <c r="K12" s="70" t="s">
+      <c r="K12" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="L12" s="55">
+      <c r="L12" s="48">
         <f>C12*K12</f>
         <v>2.6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="49">
-        <f>ROW(B13) - ROW($B$9)</f>
+    <row r="13" spans="1:13" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="42">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="44">
         <v>1</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="68" t="s">
+      <c r="E13" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="F13" s="68" t="s">
+      <c r="F13" s="59" t="s">
         <v>162</v>
       </c>
-      <c r="G13" s="68" t="s">
+      <c r="G13" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="H13" s="68" t="s">
+      <c r="H13" s="59" t="s">
         <v>246</v>
       </c>
-      <c r="I13" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J13" s="68" t="s">
+      <c r="I13" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J13" s="59" t="s">
         <v>309</v>
       </c>
-      <c r="K13" s="71" t="s">
+      <c r="K13" s="62" t="s">
         <v>368</v>
       </c>
-      <c r="L13" s="57">
-        <f t="shared" ref="L13" si="1">C13*K13</f>
+      <c r="L13" s="50">
+        <f t="shared" ref="L13" si="2">C13*K13</f>
         <v>0.24</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="48">
-        <f>ROW(B14) - ROW($B$9)</f>
+      <c r="A14" s="12"/>
+      <c r="B14" s="41">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="50">
+      <c r="C14" s="43">
         <v>1</v>
       </c>
-      <c r="D14" s="67" t="s">
+      <c r="D14" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="69" t="s">
+      <c r="F14" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="G14" s="69" t="s">
+      <c r="G14" s="60" t="s">
         <v>220</v>
       </c>
-      <c r="H14" s="69" t="s">
+      <c r="H14" s="60" t="s">
         <v>247</v>
       </c>
-      <c r="I14" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J14" s="69" t="s">
+      <c r="I14" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J14" s="60" t="s">
         <v>310</v>
       </c>
-      <c r="K14" s="70" t="s">
+      <c r="K14" s="61" t="s">
         <v>366</v>
       </c>
-      <c r="L14" s="55">
+      <c r="L14" s="48">
         <f>C14*K14</f>
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="49">
-        <f>ROW(B15) - ROW($B$9)</f>
+    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="42">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C15" s="44">
         <v>2</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="D15" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="68" t="s">
+      <c r="E15" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="F15" s="68" t="s">
+      <c r="F15" s="59" t="s">
         <v>164</v>
       </c>
-      <c r="G15" s="68" t="s">
+      <c r="G15" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="H15" s="68" t="s">
+      <c r="H15" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="I15" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J15" s="68" t="s">
+      <c r="I15" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J15" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="K15" s="71" t="s">
+      <c r="K15" s="62" t="s">
         <v>369</v>
       </c>
-      <c r="L15" s="57">
-        <f t="shared" ref="L15" si="2">C15*K15</f>
+      <c r="L15" s="50">
+        <f t="shared" ref="L15" si="3">C15*K15</f>
         <v>0.54</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="48">
-        <f>ROW(B16) - ROW($B$9)</f>
+      <c r="A16" s="12"/>
+      <c r="B16" s="41">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="43">
         <v>3</v>
       </c>
-      <c r="D16" s="67" t="s">
+      <c r="D16" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="69" t="s">
+      <c r="F16" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="G16" s="69" t="s">
+      <c r="G16" s="60" t="s">
         <v>220</v>
       </c>
-      <c r="H16" s="69" t="s">
+      <c r="H16" s="60" t="s">
         <v>249</v>
       </c>
-      <c r="I16" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J16" s="69" t="s">
+      <c r="I16" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J16" s="60" t="s">
         <v>312</v>
       </c>
-      <c r="K16" s="70" t="s">
+      <c r="K16" s="61" t="s">
         <v>370</v>
       </c>
-      <c r="L16" s="55">
+      <c r="L16" s="48">
         <f>C16*K16</f>
         <v>17.04</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="49">
-        <f>ROW(B17) - ROW($B$9)</f>
+    <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="42">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="44">
         <v>2</v>
       </c>
-      <c r="D17" s="68" t="s">
+      <c r="D17" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="68" t="s">
+      <c r="E17" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="68" t="s">
+      <c r="F17" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="G17" s="68" t="s">
+      <c r="G17" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="H17" s="68" t="s">
+      <c r="H17" s="59" t="s">
         <v>250</v>
       </c>
-      <c r="I17" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J17" s="68" t="s">
+      <c r="I17" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J17" s="59" t="s">
         <v>313</v>
       </c>
-      <c r="K17" s="71" t="s">
+      <c r="K17" s="62" t="s">
         <v>371</v>
       </c>
-      <c r="L17" s="57">
-        <f t="shared" ref="L17" si="3">C17*K17</f>
+      <c r="L17" s="50">
+        <f t="shared" ref="L17" si="4">C17*K17</f>
         <v>0.36</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="48">
-        <f>ROW(B18) - ROW($B$9)</f>
+      <c r="A18" s="12"/>
+      <c r="B18" s="41">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="50">
+      <c r="C18" s="43">
         <v>9</v>
       </c>
-      <c r="D18" s="67" t="s">
+      <c r="D18" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="E18" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="69" t="s">
+      <c r="F18" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="G18" s="69" t="s">
+      <c r="G18" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="H18" s="69" t="s">
+      <c r="H18" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="I18" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J18" s="69" t="s">
+      <c r="I18" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J18" s="60" t="s">
         <v>314</v>
       </c>
-      <c r="K18" s="70" t="s">
+      <c r="K18" s="61" t="s">
         <v>372</v>
       </c>
-      <c r="L18" s="55">
+      <c r="L18" s="48">
         <f>C18*K18</f>
         <v>1.44</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="49">
-        <f>ROW(B19) - ROW($B$9)</f>
+    <row r="19" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="42">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="51">
+      <c r="C19" s="44">
         <v>1</v>
       </c>
-      <c r="D19" s="68" t="s">
+      <c r="D19" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="68" t="s">
+      <c r="E19" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="F19" s="68" t="s">
+      <c r="F19" s="59" t="s">
         <v>168</v>
       </c>
-      <c r="G19" s="68" t="s">
+      <c r="G19" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="H19" s="68" t="s">
+      <c r="H19" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="I19" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J19" s="68" t="s">
+      <c r="I19" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J19" s="59" t="s">
         <v>315</v>
       </c>
-      <c r="K19" s="71" t="s">
+      <c r="K19" s="62" t="s">
         <v>373</v>
       </c>
-      <c r="L19" s="57">
-        <f t="shared" ref="L19" si="4">C19*K19</f>
+      <c r="L19" s="50">
+        <f t="shared" ref="L19" si="5">C19*K19</f>
         <v>0.15</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="48">
-        <f>ROW(B20) - ROW($B$9)</f>
+      <c r="A20" s="12"/>
+      <c r="B20" s="41">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="50">
+      <c r="C20" s="43">
         <v>1</v>
       </c>
-      <c r="D20" s="67" t="s">
+      <c r="D20" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="67" t="s">
+      <c r="E20" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="F20" s="69" t="s">
+      <c r="F20" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="G20" s="69" t="s">
+      <c r="G20" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="H20" s="69" t="s">
+      <c r="H20" s="60" t="s">
         <v>253</v>
       </c>
-      <c r="I20" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J20" s="69" t="s">
+      <c r="I20" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J20" s="60" t="s">
         <v>316</v>
       </c>
-      <c r="K20" s="70" t="s">
+      <c r="K20" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="L20" s="55">
+      <c r="L20" s="48">
         <f>C20*K20</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="49">
-        <f>ROW(B21) - ROW($B$9)</f>
+    <row r="21" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="42">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="51">
+      <c r="C21" s="44">
         <v>1</v>
       </c>
-      <c r="D21" s="68" t="s">
+      <c r="D21" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="68" t="s">
+      <c r="E21" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="F21" s="68" t="s">
+      <c r="F21" s="59" t="s">
         <v>170</v>
       </c>
-      <c r="G21" s="68" t="s">
+      <c r="G21" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="H21" s="68" t="s">
+      <c r="H21" s="59" t="s">
         <v>254</v>
       </c>
-      <c r="I21" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J21" s="68" t="s">
+      <c r="I21" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J21" s="59" t="s">
         <v>317</v>
       </c>
-      <c r="K21" s="71" t="s">
+      <c r="K21" s="62" t="s">
         <v>373</v>
       </c>
-      <c r="L21" s="57">
-        <f t="shared" ref="L21" si="5">C21*K21</f>
+      <c r="L21" s="50">
+        <f t="shared" ref="L21" si="6">C21*K21</f>
         <v>0.15</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="48">
-        <f>ROW(B22) - ROW($B$9)</f>
+      <c r="A22" s="12"/>
+      <c r="B22" s="41">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="50">
+      <c r="C22" s="43">
         <v>8</v>
       </c>
-      <c r="D22" s="67" t="s">
+      <c r="D22" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="67" t="s">
+      <c r="E22" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="F22" s="69" t="s">
+      <c r="F22" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="G22" s="69" t="s">
+      <c r="G22" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="H22" s="69" t="s">
+      <c r="H22" s="60" t="s">
         <v>255</v>
       </c>
-      <c r="I22" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J22" s="69" t="s">
+      <c r="I22" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J22" s="60" t="s">
         <v>318</v>
       </c>
-      <c r="K22" s="70" t="s">
+      <c r="K22" s="61" t="s">
         <v>375</v>
       </c>
-      <c r="L22" s="55">
+      <c r="L22" s="48">
         <f>C22*K22</f>
         <v>0.96</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="49">
-        <f>ROW(B23) - ROW($B$9)</f>
+    <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="42">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="51">
+      <c r="C23" s="44">
         <v>4</v>
       </c>
-      <c r="D23" s="68" t="s">
+      <c r="D23" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="68" t="s">
+      <c r="E23" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="68" t="s">
+      <c r="F23" s="59" t="s">
         <v>172</v>
       </c>
-      <c r="G23" s="68" t="s">
+      <c r="G23" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="H23" s="68" t="s">
+      <c r="H23" s="59" t="s">
         <v>256</v>
       </c>
-      <c r="I23" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J23" s="68" t="s">
+      <c r="I23" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J23" s="59" t="s">
         <v>319</v>
       </c>
-      <c r="K23" s="71" t="s">
+      <c r="K23" s="62" t="s">
         <v>376</v>
       </c>
-      <c r="L23" s="57">
-        <f t="shared" ref="L23" si="6">C23*K23</f>
+      <c r="L23" s="50">
+        <f t="shared" ref="L23" si="7">C23*K23</f>
         <v>41.56</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="48">
-        <f>ROW(B24) - ROW($B$9)</f>
+      <c r="A24" s="12"/>
+      <c r="B24" s="41">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="50">
+      <c r="C24" s="43">
         <v>4</v>
       </c>
-      <c r="D24" s="67" t="s">
+      <c r="D24" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="67" t="s">
+      <c r="E24" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="F24" s="69" t="s">
+      <c r="F24" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="G24" s="69" t="s">
+      <c r="G24" s="60" t="s">
         <v>224</v>
       </c>
-      <c r="H24" s="69" t="s">
+      <c r="H24" s="60" t="s">
         <v>257</v>
       </c>
-      <c r="I24" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J24" s="69" t="s">
+      <c r="I24" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J24" s="60" t="s">
         <v>320</v>
       </c>
-      <c r="K24" s="70" t="s">
+      <c r="K24" s="61" t="s">
         <v>376</v>
       </c>
-      <c r="L24" s="55">
+      <c r="L24" s="48">
         <f>C24*K24</f>
         <v>41.56</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="49">
-        <f>ROW(B25) - ROW($B$9)</f>
+    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="42">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="51">
+      <c r="C25" s="44">
         <v>2</v>
       </c>
-      <c r="D25" s="68" t="s">
+      <c r="D25" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="68" t="s">
+      <c r="E25" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="68" t="s">
+      <c r="F25" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="G25" s="68" t="s">
+      <c r="G25" s="59" t="s">
         <v>225</v>
       </c>
-      <c r="H25" s="68" t="s">
+      <c r="H25" s="59" t="s">
         <v>258</v>
       </c>
-      <c r="I25" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J25" s="68" t="s">
+      <c r="I25" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J25" s="59" t="s">
         <v>321</v>
       </c>
-      <c r="K25" s="71" t="s">
+      <c r="K25" s="62" t="s">
         <v>377</v>
       </c>
-      <c r="L25" s="57">
-        <f t="shared" ref="L25" si="7">C25*K25</f>
+      <c r="L25" s="50">
+        <f t="shared" ref="L25" si="8">C25*K25</f>
         <v>2.8</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="48">
-        <f>ROW(B26) - ROW($B$9)</f>
+      <c r="A26" s="12"/>
+      <c r="B26" s="41">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="50">
+      <c r="C26" s="43">
         <v>1</v>
       </c>
-      <c r="D26" s="67" t="s">
+      <c r="D26" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="67" t="s">
+      <c r="E26" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="69" t="s">
+      <c r="F26" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="G26" s="69" t="s">
+      <c r="G26" s="60" t="s">
         <v>226</v>
       </c>
-      <c r="H26" s="69" t="s">
+      <c r="H26" s="60" t="s">
         <v>259</v>
       </c>
-      <c r="I26" s="69" t="s">
+      <c r="I26" s="60" t="s">
         <v>304</v>
       </c>
-      <c r="J26" s="69" t="s">
+      <c r="J26" s="60" t="s">
         <v>322</v>
       </c>
-      <c r="K26" s="70" t="s">
+      <c r="K26" s="61" t="s">
         <v>378</v>
       </c>
-      <c r="L26" s="55">
+      <c r="L26" s="48">
         <f>C26*K26</f>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="49">
-        <f>ROW(B27) - ROW($B$9)</f>
+    <row r="27" spans="1:12" s="82" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="81"/>
+      <c r="B27" s="42">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="51">
+      <c r="C27" s="44">
         <v>10</v>
       </c>
-      <c r="D27" s="68" t="s">
+      <c r="D27" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="68" t="s">
+      <c r="E27" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="F27" s="68" t="s">
+      <c r="F27" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="G27" s="68" t="s">
+      <c r="G27" s="59" t="s">
         <v>226</v>
       </c>
-      <c r="H27" s="68" t="s">
+      <c r="H27" s="59" t="s">
         <v>260</v>
       </c>
-      <c r="I27" s="68" t="s">
+      <c r="I27" s="59" t="s">
         <v>304</v>
       </c>
-      <c r="J27" s="68" t="s">
+      <c r="J27" s="59" t="s">
         <v>323</v>
       </c>
-      <c r="K27" s="71" t="s">
+      <c r="K27" s="62" t="s">
         <v>378</v>
       </c>
-      <c r="L27" s="57">
-        <f t="shared" ref="L27" si="8">C27*K27</f>
+      <c r="L27" s="50">
+        <f t="shared" ref="L27" si="9">C27*K27</f>
         <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="48">
-        <f>ROW(B28) - ROW($B$9)</f>
+      <c r="A28" s="12"/>
+      <c r="B28" s="41">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="50">
+      <c r="C28" s="43">
         <v>1</v>
       </c>
-      <c r="D28" s="67" t="s">
+      <c r="D28" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="67" t="s">
+      <c r="E28" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="F28" s="69" t="s">
+      <c r="F28" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="G28" s="69" t="s">
+      <c r="G28" s="60" t="s">
         <v>227</v>
       </c>
-      <c r="H28" s="69" t="s">
+      <c r="H28" s="60" t="s">
         <v>261</v>
       </c>
-      <c r="I28" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J28" s="69" t="s">
+      <c r="I28" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J28" s="60" t="s">
         <v>324</v>
       </c>
-      <c r="K28" s="70" t="s">
+      <c r="K28" s="61" t="s">
         <v>379</v>
       </c>
-      <c r="L28" s="55">
+      <c r="L28" s="48">
         <f>C28*K28</f>
         <v>0.48</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="49">
-        <f>ROW(B29) - ROW($B$9)</f>
+    <row r="29" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+      <c r="B29" s="42">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="51">
+      <c r="C29" s="44">
         <v>2</v>
       </c>
-      <c r="D29" s="68" t="s">
+      <c r="D29" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="68" t="s">
+      <c r="E29" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="F29" s="68" t="s">
+      <c r="F29" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="G29" s="68" t="s">
+      <c r="G29" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="H29" s="68" t="s">
+      <c r="H29" s="59" t="s">
         <v>262</v>
       </c>
-      <c r="I29" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J29" s="68" t="s">
+      <c r="I29" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J29" s="59" t="s">
         <v>325</v>
       </c>
-      <c r="K29" s="71" t="s">
+      <c r="K29" s="62" t="s">
         <v>380</v>
       </c>
-      <c r="L29" s="57">
-        <f t="shared" ref="L29" si="9">C29*K29</f>
+      <c r="L29" s="50">
+        <f t="shared" ref="L29" si="10">C29*K29</f>
         <v>2.14</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="48">
-        <f>ROW(B30) - ROW($B$9)</f>
+      <c r="A30" s="12"/>
+      <c r="B30" s="41">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="50">
+      <c r="C30" s="43">
         <v>7</v>
       </c>
-      <c r="D30" s="67" t="s">
+      <c r="D30" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="67" t="s">
+      <c r="E30" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="F30" s="69" t="s">
+      <c r="F30" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="G30" s="69" t="s">
+      <c r="G30" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="H30" s="69" t="s">
+      <c r="H30" s="60" t="s">
         <v>263</v>
       </c>
-      <c r="I30" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J30" s="69" t="s">
+      <c r="I30" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J30" s="60" t="s">
         <v>326</v>
       </c>
-      <c r="K30" s="70" t="s">
+      <c r="K30" s="61" t="s">
         <v>381</v>
       </c>
-      <c r="L30" s="55">
+      <c r="L30" s="48">
         <f>C30*K30</f>
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="49">
-        <f>ROW(B31) - ROW($B$9)</f>
+    <row r="31" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="12"/>
+      <c r="B31" s="42">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C31" s="51">
+      <c r="C31" s="44">
         <v>1</v>
       </c>
-      <c r="D31" s="68" t="s">
+      <c r="D31" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="68" t="s">
+      <c r="E31" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="F31" s="68" t="s">
+      <c r="F31" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="G31" s="68" t="s">
+      <c r="G31" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="H31" s="68" t="s">
+      <c r="H31" s="59" t="s">
         <v>264</v>
       </c>
-      <c r="I31" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J31" s="68" t="s">
+      <c r="I31" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J31" s="59" t="s">
         <v>327</v>
       </c>
-      <c r="K31" s="71" t="s">
+      <c r="K31" s="62" t="s">
         <v>382</v>
       </c>
-      <c r="L31" s="57">
-        <f t="shared" ref="L31" si="10">C31*K31</f>
+      <c r="L31" s="50">
+        <f t="shared" ref="L31" si="11">C31*K31</f>
         <v>1.36</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="48">
-        <f>ROW(B32) - ROW($B$9)</f>
+      <c r="A32" s="12"/>
+      <c r="B32" s="41">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C32" s="50">
+      <c r="C32" s="43">
         <v>8</v>
       </c>
-      <c r="D32" s="67" t="s">
+      <c r="D32" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="67" t="s">
+      <c r="E32" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="F32" s="69" t="s">
+      <c r="F32" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="G32" s="69" t="s">
+      <c r="G32" s="60" t="s">
         <v>228</v>
       </c>
-      <c r="H32" s="69" t="s">
+      <c r="H32" s="60" t="s">
         <v>265</v>
       </c>
-      <c r="I32" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J32" s="69" t="s">
+      <c r="I32" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J32" s="60" t="s">
         <v>328</v>
       </c>
-      <c r="K32" s="70" t="s">
+      <c r="K32" s="61" t="s">
         <v>383</v>
       </c>
-      <c r="L32" s="55">
+      <c r="L32" s="48">
         <f>C32*K32</f>
         <v>12.72</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="49">
-        <f>ROW(B33) - ROW($B$9)</f>
+    <row r="33" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="12"/>
+      <c r="B33" s="42">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C33" s="51">
+      <c r="C33" s="44">
         <v>10</v>
       </c>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="E33" s="68" t="s">
+      <c r="E33" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="F33" s="68" t="s">
+      <c r="F33" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="G33" s="68" t="s">
+      <c r="G33" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="H33" s="68" t="s">
+      <c r="H33" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="I33" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J33" s="68" t="s">
+      <c r="I33" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J33" s="59" t="s">
         <v>329</v>
       </c>
-      <c r="K33" s="71" t="s">
+      <c r="K33" s="62" t="s">
         <v>384</v>
       </c>
-      <c r="L33" s="57">
-        <f t="shared" ref="L33" si="11">C33*K33</f>
+      <c r="L33" s="50">
+        <f t="shared" ref="L33" si="12">C33*K33</f>
         <v>1.3</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="48">
-        <f>ROW(B34) - ROW($B$9)</f>
+      <c r="A34" s="12"/>
+      <c r="B34" s="41">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C34" s="50">
+      <c r="C34" s="43">
         <v>10</v>
       </c>
-      <c r="D34" s="67" t="s">
+      <c r="D34" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="67" t="s">
+      <c r="E34" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="60" t="s">
         <v>183</v>
       </c>
-      <c r="G34" s="69" t="s">
+      <c r="G34" s="60" t="s">
         <v>229</v>
       </c>
-      <c r="H34" s="69" t="s">
+      <c r="H34" s="60" t="s">
         <v>267</v>
       </c>
-      <c r="I34" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J34" s="69" t="s">
+      <c r="I34" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J34" s="60" t="s">
         <v>330</v>
       </c>
-      <c r="K34" s="70" t="s">
+      <c r="K34" s="61" t="s">
         <v>384</v>
       </c>
-      <c r="L34" s="55">
+      <c r="L34" s="48">
         <f>C34*K34</f>
         <v>1.3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="49">
-        <f>ROW(B35) - ROW($B$9)</f>
+    <row r="35" spans="1:12" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A35" s="12"/>
+      <c r="B35" s="42">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C35" s="51">
+      <c r="C35" s="44">
         <v>8</v>
       </c>
-      <c r="D35" s="68" t="s">
+      <c r="D35" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="68" t="s">
+      <c r="E35" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="F35" s="68" t="s">
+      <c r="F35" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="G35" s="68" t="s">
+      <c r="G35" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="H35" s="68" t="s">
+      <c r="H35" s="59" t="s">
         <v>268</v>
       </c>
-      <c r="I35" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J35" s="68" t="s">
+      <c r="I35" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J35" s="59" t="s">
         <v>331</v>
       </c>
-      <c r="K35" s="71" t="s">
+      <c r="K35" s="62" t="s">
         <v>385</v>
       </c>
-      <c r="L35" s="57">
-        <f t="shared" ref="L35" si="12">C35*K35</f>
+      <c r="L35" s="50">
+        <f t="shared" ref="L35" si="13">C35*K35</f>
         <v>14.08</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="48">
-        <f>ROW(B36) - ROW($B$9)</f>
+      <c r="A36" s="12"/>
+      <c r="B36" s="41">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C36" s="50">
+      <c r="C36" s="43">
         <v>2</v>
       </c>
-      <c r="D36" s="67" t="s">
+      <c r="D36" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="67" t="s">
+      <c r="E36" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="F36" s="69" t="s">
+      <c r="F36" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="G36" s="69" t="s">
+      <c r="G36" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H36" s="69" t="s">
+      <c r="H36" s="60" t="s">
         <v>269</v>
       </c>
-      <c r="I36" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J36" s="69" t="s">
+      <c r="I36" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J36" s="60" t="s">
         <v>332</v>
       </c>
-      <c r="K36" s="70" t="s">
+      <c r="K36" s="61" t="s">
         <v>386</v>
       </c>
-      <c r="L36" s="55">
+      <c r="L36" s="48">
         <f>C36*K36</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="49">
-        <f>ROW(B37) - ROW($B$9)</f>
+    <row r="37" spans="1:12" s="3" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="42">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C37" s="51">
+      <c r="C37" s="44">
         <v>27</v>
       </c>
-      <c r="D37" s="68" t="s">
+      <c r="D37" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="68" t="s">
+      <c r="E37" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="F37" s="68" t="s">
+      <c r="F37" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="G37" s="68" t="s">
+      <c r="G37" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="H37" s="68" t="s">
+      <c r="H37" s="59" t="s">
         <v>270</v>
       </c>
-      <c r="I37" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J37" s="68" t="s">
+      <c r="I37" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J37" s="59" t="s">
         <v>333</v>
       </c>
-      <c r="K37" s="71" t="s">
+      <c r="K37" s="62" t="s">
         <v>387</v>
       </c>
-      <c r="L37" s="57">
-        <f t="shared" ref="L37" si="13">C37*K37</f>
+      <c r="L37" s="50">
+        <f t="shared" ref="L37" si="14">C37*K37</f>
         <v>2.7</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="48">
-        <f>ROW(B38) - ROW($B$9)</f>
+      <c r="A38" s="12"/>
+      <c r="B38" s="41">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C38" s="50">
+      <c r="C38" s="43">
         <v>2</v>
       </c>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="67" t="s">
+      <c r="E38" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="F38" s="69" t="s">
+      <c r="F38" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="G38" s="69" t="s">
+      <c r="G38" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H38" s="69" t="s">
+      <c r="H38" s="60" t="s">
         <v>271</v>
       </c>
-      <c r="I38" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J38" s="69" t="s">
+      <c r="I38" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J38" s="60" t="s">
         <v>334</v>
       </c>
-      <c r="K38" s="70" t="s">
+      <c r="K38" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="L38" s="55">
+      <c r="L38" s="48">
         <f>C38*K38</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="49">
-        <f>ROW(B39) - ROW($B$9)</f>
+    <row r="39" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="42">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C39" s="51">
+      <c r="C39" s="44">
         <v>2</v>
       </c>
-      <c r="D39" s="68" t="s">
+      <c r="D39" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="E39" s="68" t="s">
+      <c r="E39" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="F39" s="68" t="s">
+      <c r="F39" s="59" t="s">
         <v>188</v>
       </c>
-      <c r="G39" s="68" t="s">
+      <c r="G39" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="H39" s="68" t="s">
+      <c r="H39" s="59" t="s">
         <v>272</v>
       </c>
-      <c r="I39" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J39" s="68" t="s">
+      <c r="I39" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J39" s="59" t="s">
         <v>335</v>
       </c>
-      <c r="K39" s="71" t="s">
+      <c r="K39" s="62" t="s">
         <v>367</v>
       </c>
-      <c r="L39" s="57">
-        <f t="shared" ref="L39" si="14">C39*K39</f>
+      <c r="L39" s="50">
+        <f t="shared" ref="L39" si="15">C39*K39</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="48">
-        <f>ROW(B40) - ROW($B$9)</f>
+      <c r="A40" s="12"/>
+      <c r="B40" s="41">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C40" s="50">
+      <c r="C40" s="43">
         <v>1</v>
       </c>
-      <c r="D40" s="67" t="s">
+      <c r="D40" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E40" s="67" t="s">
+      <c r="E40" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="F40" s="69" t="s">
+      <c r="F40" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="G40" s="69" t="s">
+      <c r="G40" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H40" s="69" t="s">
+      <c r="H40" s="60" t="s">
         <v>273</v>
       </c>
-      <c r="I40" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J40" s="69" t="s">
+      <c r="I40" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J40" s="60" t="s">
         <v>336</v>
       </c>
-      <c r="K40" s="70" t="s">
+      <c r="K40" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="L40" s="55">
+      <c r="L40" s="48">
         <f>C40*K40</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="49">
-        <f>ROW(B41) - ROW($B$9)</f>
+    <row r="41" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="12"/>
+      <c r="B41" s="42">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="C41" s="51">
+      <c r="C41" s="44">
         <v>7</v>
       </c>
-      <c r="D41" s="68" t="s">
+      <c r="D41" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="E41" s="68" t="s">
+      <c r="E41" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="F41" s="68" t="s">
+      <c r="F41" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="G41" s="68" t="s">
+      <c r="G41" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="H41" s="68" t="s">
+      <c r="H41" s="59" t="s">
         <v>274</v>
       </c>
-      <c r="I41" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J41" s="68" t="s">
+      <c r="I41" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J41" s="59" t="s">
         <v>337</v>
       </c>
-      <c r="K41" s="71" t="s">
+      <c r="K41" s="62" t="s">
         <v>367</v>
       </c>
-      <c r="L41" s="57">
-        <f t="shared" ref="L41" si="15">C41*K41</f>
+      <c r="L41" s="50">
+        <f t="shared" ref="L41" si="16">C41*K41</f>
         <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="48">
-        <f>ROW(B42) - ROW($B$9)</f>
+      <c r="A42" s="12"/>
+      <c r="B42" s="41">
+        <f t="shared" ref="B42:B68" si="17">ROW(B42) - ROW($B$9)</f>
         <v>33</v>
       </c>
-      <c r="C42" s="50">
+      <c r="C42" s="43">
         <v>1</v>
       </c>
-      <c r="D42" s="67" t="s">
+      <c r="D42" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="E42" s="67" t="s">
+      <c r="E42" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="F42" s="69" t="s">
+      <c r="F42" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="G42" s="69" t="s">
+      <c r="G42" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H42" s="69" t="s">
+      <c r="H42" s="60" t="s">
         <v>275</v>
       </c>
-      <c r="I42" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J42" s="69" t="s">
+      <c r="I42" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J42" s="60" t="s">
         <v>338</v>
       </c>
-      <c r="K42" s="70" t="s">
+      <c r="K42" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="L42" s="55">
+      <c r="L42" s="48">
         <f>C42*K42</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="49">
-        <f>ROW(B43) - ROW($B$9)</f>
+    <row r="43" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="12"/>
+      <c r="B43" s="42">
+        <f t="shared" si="17"/>
         <v>34</v>
       </c>
-      <c r="C43" s="51">
+      <c r="C43" s="44">
         <v>1</v>
       </c>
-      <c r="D43" s="68" t="s">
+      <c r="D43" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="E43" s="68" t="s">
+      <c r="E43" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="F43" s="68" t="s">
+      <c r="F43" s="59" t="s">
         <v>192</v>
       </c>
-      <c r="G43" s="68" t="s">
+      <c r="G43" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="H43" s="68" t="s">
+      <c r="H43" s="59" t="s">
         <v>276</v>
       </c>
-      <c r="I43" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J43" s="68" t="s">
+      <c r="I43" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J43" s="59" t="s">
         <v>339</v>
       </c>
-      <c r="K43" s="71" t="s">
+      <c r="K43" s="62" t="s">
         <v>384</v>
       </c>
-      <c r="L43" s="57">
-        <f t="shared" ref="L43" si="16">C43*K43</f>
+      <c r="L43" s="50">
+        <f t="shared" ref="L43" si="18">C43*K43</f>
         <v>0.13</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="48">
-        <f>ROW(B44) - ROW($B$9)</f>
+      <c r="A44" s="12"/>
+      <c r="B44" s="41">
+        <f t="shared" si="17"/>
         <v>35</v>
       </c>
-      <c r="C44" s="50">
+      <c r="C44" s="43">
         <v>1</v>
       </c>
-      <c r="D44" s="67" t="s">
+      <c r="D44" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="E44" s="67" t="s">
+      <c r="E44" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="F44" s="69" t="s">
+      <c r="F44" s="60" t="s">
         <v>193</v>
       </c>
-      <c r="G44" s="69" t="s">
+      <c r="G44" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H44" s="69" t="s">
+      <c r="H44" s="60" t="s">
         <v>277</v>
       </c>
-      <c r="I44" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J44" s="69" t="s">
+      <c r="I44" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J44" s="60" t="s">
         <v>340</v>
       </c>
-      <c r="K44" s="70" t="s">
+      <c r="K44" s="61" t="s">
         <v>387</v>
       </c>
-      <c r="L44" s="55">
+      <c r="L44" s="48">
         <f>C44*K44</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="49">
-        <f>ROW(B45) - ROW($B$9)</f>
+    <row r="45" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="12"/>
+      <c r="B45" s="42">
+        <f t="shared" si="17"/>
         <v>36</v>
       </c>
-      <c r="C45" s="51">
+      <c r="C45" s="44">
         <v>8</v>
       </c>
-      <c r="D45" s="68" t="s">
+      <c r="D45" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="E45" s="68" t="s">
+      <c r="E45" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="F45" s="68" t="s">
+      <c r="F45" s="59" t="s">
         <v>194</v>
       </c>
-      <c r="G45" s="68" t="s">
+      <c r="G45" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="H45" s="68" t="s">
+      <c r="H45" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="I45" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J45" s="68" t="s">
+      <c r="I45" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J45" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="K45" s="71" t="s">
+      <c r="K45" s="62" t="s">
         <v>388</v>
       </c>
-      <c r="L45" s="57">
-        <f t="shared" ref="L45" si="17">C45*K45</f>
+      <c r="L45" s="50">
+        <f t="shared" ref="L45" si="19">C45*K45</f>
         <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="48">
-        <f>ROW(B46) - ROW($B$9)</f>
+      <c r="A46" s="12"/>
+      <c r="B46" s="41">
+        <f t="shared" si="17"/>
         <v>37</v>
       </c>
-      <c r="C46" s="50">
+      <c r="C46" s="43">
         <v>2</v>
       </c>
-      <c r="D46" s="67" t="s">
+      <c r="D46" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="67" t="s">
+      <c r="E46" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="F46" s="69" t="s">
+      <c r="F46" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="G46" s="69" t="s">
+      <c r="G46" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H46" s="69" t="s">
+      <c r="H46" s="60" t="s">
         <v>279</v>
       </c>
-      <c r="I46" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J46" s="69" t="s">
+      <c r="I46" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J46" s="60" t="s">
         <v>342</v>
       </c>
-      <c r="K46" s="70" t="s">
+      <c r="K46" s="61" t="s">
         <v>387</v>
       </c>
-      <c r="L46" s="55">
+      <c r="L46" s="48">
         <f>C46*K46</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="49">
-        <f>ROW(B47) - ROW($B$9)</f>
+    <row r="47" spans="1:12" s="3" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="12"/>
+      <c r="B47" s="42">
+        <f t="shared" si="17"/>
         <v>38</v>
       </c>
-      <c r="C47" s="51">
+      <c r="C47" s="44">
         <v>16</v>
       </c>
-      <c r="D47" s="68" t="s">
+      <c r="D47" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="E47" s="68" t="s">
+      <c r="E47" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="F47" s="68" t="s">
+      <c r="F47" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="G47" s="68" t="s">
+      <c r="G47" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="H47" s="68" t="s">
+      <c r="H47" s="59" t="s">
         <v>280</v>
       </c>
-      <c r="I47" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J47" s="68" t="s">
+      <c r="I47" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J47" s="59" t="s">
         <v>339</v>
       </c>
-      <c r="K47" s="71" t="s">
+      <c r="K47" s="62" t="s">
         <v>389</v>
       </c>
-      <c r="L47" s="57">
-        <f t="shared" ref="L47" si="18">C47*K47</f>
+      <c r="L47" s="50">
+        <f t="shared" ref="L47" si="20">C47*K47</f>
         <v>7.2</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="48">
-        <f>ROW(B48) - ROW($B$9)</f>
+      <c r="A48" s="12"/>
+      <c r="B48" s="41">
+        <f t="shared" si="17"/>
         <v>39</v>
       </c>
-      <c r="C48" s="50">
+      <c r="C48" s="43">
         <v>2</v>
       </c>
-      <c r="D48" s="67" t="s">
+      <c r="D48" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="E48" s="67" t="s">
+      <c r="E48" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="F48" s="69" t="s">
+      <c r="F48" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="G48" s="69" t="s">
+      <c r="G48" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H48" s="69" t="s">
+      <c r="H48" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="I48" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J48" s="69" t="s">
+      <c r="I48" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J48" s="60" t="s">
         <v>343</v>
       </c>
-      <c r="K48" s="70" t="s">
+      <c r="K48" s="61" t="s">
         <v>366</v>
       </c>
-      <c r="L48" s="55">
+      <c r="L48" s="48">
         <f>C48*K48</f>
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="49">
-        <f>ROW(B49) - ROW($B$9)</f>
+    <row r="49" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="12"/>
+      <c r="B49" s="42">
+        <f t="shared" si="17"/>
         <v>40</v>
       </c>
-      <c r="C49" s="51">
+      <c r="C49" s="44">
         <v>2</v>
       </c>
-      <c r="D49" s="68" t="s">
+      <c r="D49" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="E49" s="68" t="s">
+      <c r="E49" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="F49" s="68" t="s">
+      <c r="F49" s="59" t="s">
         <v>198</v>
       </c>
-      <c r="G49" s="68" t="s">
+      <c r="G49" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="H49" s="68" t="s">
+      <c r="H49" s="59" t="s">
         <v>282</v>
       </c>
-      <c r="I49" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J49" s="68" t="s">
+      <c r="I49" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J49" s="59" t="s">
         <v>344</v>
       </c>
-      <c r="K49" s="71" t="s">
+      <c r="K49" s="62" t="s">
         <v>390</v>
       </c>
-      <c r="L49" s="57">
-        <f t="shared" ref="L49" si="19">C49*K49</f>
+      <c r="L49" s="50">
+        <f t="shared" ref="L49" si="21">C49*K49</f>
         <v>0.42</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="48">
-        <f>ROW(B50) - ROW($B$9)</f>
+      <c r="A50" s="12"/>
+      <c r="B50" s="41">
+        <f t="shared" si="17"/>
         <v>41</v>
       </c>
-      <c r="C50" s="50">
+      <c r="C50" s="43">
         <v>1</v>
       </c>
-      <c r="D50" s="67" t="s">
+      <c r="D50" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="E50" s="67" t="s">
+      <c r="E50" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="F50" s="69" t="s">
+      <c r="F50" s="60" t="s">
         <v>199</v>
       </c>
-      <c r="G50" s="69" t="s">
+      <c r="G50" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H50" s="69" t="s">
+      <c r="H50" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="I50" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J50" s="69" t="s">
+      <c r="I50" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J50" s="60" t="s">
         <v>345</v>
       </c>
-      <c r="K50" s="70" t="s">
+      <c r="K50" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="L50" s="55">
+      <c r="L50" s="48">
         <f>C50*K50</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="49">
-        <f>ROW(B51) - ROW($B$9)</f>
+    <row r="51" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="12"/>
+      <c r="B51" s="42">
+        <f t="shared" si="17"/>
         <v>42</v>
       </c>
-      <c r="C51" s="51">
+      <c r="C51" s="44">
         <v>1</v>
       </c>
-      <c r="D51" s="68" t="s">
+      <c r="D51" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="E51" s="68" t="s">
+      <c r="E51" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="F51" s="68" t="s">
+      <c r="F51" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="G51" s="68" t="s">
+      <c r="G51" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="H51" s="68" t="s">
+      <c r="H51" s="59" t="s">
         <v>284</v>
       </c>
-      <c r="I51" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J51" s="68" t="s">
+      <c r="I51" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J51" s="59" t="s">
         <v>346</v>
       </c>
-      <c r="K51" s="71" t="s">
+      <c r="K51" s="62" t="s">
         <v>367</v>
       </c>
-      <c r="L51" s="57">
-        <f t="shared" ref="L51" si="20">C51*K51</f>
+      <c r="L51" s="50">
+        <f t="shared" ref="L51" si="22">C51*K51</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="48">
-        <f>ROW(B52) - ROW($B$9)</f>
+      <c r="A52" s="12"/>
+      <c r="B52" s="41">
+        <f t="shared" si="17"/>
         <v>43</v>
       </c>
-      <c r="C52" s="50">
+      <c r="C52" s="43">
         <v>1</v>
       </c>
-      <c r="D52" s="67" t="s">
+      <c r="D52" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="E52" s="67" t="s">
+      <c r="E52" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="F52" s="69" t="s">
+      <c r="F52" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="G52" s="69" t="s">
+      <c r="G52" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H52" s="69" t="s">
+      <c r="H52" s="60" t="s">
         <v>285</v>
       </c>
-      <c r="I52" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J52" s="69" t="s">
+      <c r="I52" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J52" s="60" t="s">
         <v>347</v>
       </c>
-      <c r="K52" s="70" t="s">
+      <c r="K52" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="L52" s="55">
+      <c r="L52" s="48">
         <f>C52*K52</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
-      <c r="B53" s="49">
-        <f>ROW(B53) - ROW($B$9)</f>
+    <row r="53" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="12"/>
+      <c r="B53" s="42">
+        <f t="shared" si="17"/>
         <v>44</v>
       </c>
-      <c r="C53" s="51">
+      <c r="C53" s="44">
         <v>2</v>
       </c>
-      <c r="D53" s="68" t="s">
+      <c r="D53" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="E53" s="68" t="s">
+      <c r="E53" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="F53" s="68" t="s">
+      <c r="F53" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="G53" s="68" t="s">
+      <c r="G53" s="59" t="s">
         <v>232</v>
       </c>
-      <c r="H53" s="68" t="s">
+      <c r="H53" s="59" t="s">
         <v>286</v>
       </c>
-      <c r="I53" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J53" s="68" t="s">
+      <c r="I53" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J53" s="59" t="s">
         <v>348</v>
       </c>
-      <c r="K53" s="71" t="s">
+      <c r="K53" s="62" t="s">
         <v>391</v>
       </c>
-      <c r="L53" s="57">
-        <f t="shared" ref="L53" si="21">C53*K53</f>
+      <c r="L53" s="50">
+        <f t="shared" ref="L53" si="23">C53*K53</f>
         <v>2.46</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="48">
-        <f>ROW(B54) - ROW($B$9)</f>
+      <c r="A54" s="12"/>
+      <c r="B54" s="41">
+        <f t="shared" si="17"/>
         <v>45</v>
       </c>
-      <c r="C54" s="50">
+      <c r="C54" s="43">
         <v>4</v>
       </c>
-      <c r="D54" s="67" t="s">
+      <c r="D54" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="E54" s="67" t="s">
+      <c r="E54" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="F54" s="69" t="s">
+      <c r="F54" s="60" t="s">
         <v>203</v>
       </c>
-      <c r="G54" s="69" t="s">
+      <c r="G54" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="H54" s="69" t="s">
+      <c r="H54" s="60" t="s">
         <v>287</v>
       </c>
-      <c r="I54" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J54" s="69" t="s">
+      <c r="I54" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J54" s="60" t="s">
         <v>349</v>
       </c>
-      <c r="K54" s="70" t="s">
+      <c r="K54" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="L54" s="55">
+      <c r="L54" s="48">
         <f>C54*K54</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="49">
-        <f>ROW(B55) - ROW($B$9)</f>
+    <row r="55" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="12"/>
+      <c r="B55" s="42">
+        <f t="shared" si="17"/>
         <v>46</v>
       </c>
-      <c r="C55" s="51">
+      <c r="C55" s="44">
         <v>1</v>
       </c>
-      <c r="D55" s="68" t="s">
+      <c r="D55" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="E55" s="68" t="s">
+      <c r="E55" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="F55" s="68" t="s">
+      <c r="F55" s="59" t="s">
         <v>204</v>
       </c>
-      <c r="G55" s="68" t="s">
+      <c r="G55" s="59" t="s">
         <v>233</v>
       </c>
-      <c r="H55" s="68" t="s">
+      <c r="H55" s="59" t="s">
         <v>288</v>
       </c>
-      <c r="I55" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J55" s="68" t="s">
+      <c r="I55" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J55" s="59" t="s">
         <v>350</v>
       </c>
-      <c r="K55" s="71" t="s">
+      <c r="K55" s="62" t="s">
         <v>392</v>
       </c>
-      <c r="L55" s="57">
-        <f t="shared" ref="L55" si="22">C55*K55</f>
+      <c r="L55" s="50">
+        <f t="shared" ref="L55" si="24">C55*K55</f>
         <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="56" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="48">
-        <f>ROW(B56) - ROW($B$9)</f>
+      <c r="A56" s="12"/>
+      <c r="B56" s="41">
+        <f t="shared" si="17"/>
         <v>47</v>
       </c>
-      <c r="C56" s="50">
+      <c r="C56" s="43">
         <v>2</v>
       </c>
-      <c r="D56" s="67" t="s">
+      <c r="D56" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E56" s="67" t="s">
+      <c r="E56" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="F56" s="69" t="s">
+      <c r="F56" s="60" t="s">
         <v>205</v>
       </c>
-      <c r="G56" s="69" t="s">
+      <c r="G56" s="60" t="s">
         <v>234</v>
       </c>
-      <c r="H56" s="69" t="s">
+      <c r="H56" s="60" t="s">
         <v>289</v>
       </c>
-      <c r="I56" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J56" s="69" t="s">
+      <c r="I56" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J56" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="K56" s="70" t="s">
+      <c r="K56" s="61" t="s">
         <v>393</v>
       </c>
-      <c r="L56" s="55">
+      <c r="L56" s="48">
         <f>C56*K56</f>
         <v>7.54</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="49">
-        <f>ROW(B57) - ROW($B$9)</f>
+    <row r="57" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="12"/>
+      <c r="B57" s="42">
+        <f t="shared" si="17"/>
         <v>48</v>
       </c>
-      <c r="C57" s="51">
+      <c r="C57" s="44">
         <v>2</v>
       </c>
-      <c r="D57" s="68" t="s">
+      <c r="D57" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="E57" s="68" t="s">
+      <c r="E57" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="F57" s="68" t="s">
+      <c r="F57" s="59" t="s">
         <v>206</v>
       </c>
-      <c r="G57" s="68" t="s">
+      <c r="G57" s="59" t="s">
         <v>235</v>
       </c>
-      <c r="H57" s="68" t="s">
+      <c r="H57" s="59" t="s">
         <v>290</v>
       </c>
-      <c r="I57" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J57" s="68" t="s">
+      <c r="I57" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J57" s="59" t="s">
         <v>352</v>
       </c>
-      <c r="K57" s="71" t="s">
+      <c r="K57" s="62" t="s">
         <v>394</v>
       </c>
-      <c r="L57" s="57">
-        <f t="shared" ref="L57" si="23">C57*K57</f>
+      <c r="L57" s="50">
+        <f t="shared" ref="L57" si="25">C57*K57</f>
         <v>2.48</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="48">
-        <f>ROW(B58) - ROW($B$9)</f>
+      <c r="A58" s="12"/>
+      <c r="B58" s="41">
+        <f t="shared" si="17"/>
         <v>49</v>
       </c>
-      <c r="C58" s="50">
+      <c r="C58" s="43">
         <v>2</v>
       </c>
-      <c r="D58" s="67" t="s">
+      <c r="D58" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="E58" s="67" t="s">
+      <c r="E58" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="F58" s="69" t="s">
+      <c r="F58" s="60" t="s">
         <v>207</v>
       </c>
-      <c r="G58" s="69" t="s">
+      <c r="G58" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="H58" s="69" t="s">
+      <c r="H58" s="60" t="s">
         <v>291</v>
       </c>
-      <c r="I58" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J58" s="69" t="s">
+      <c r="I58" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J58" s="60" t="s">
         <v>353</v>
       </c>
-      <c r="K58" s="70" t="s">
+      <c r="K58" s="61" t="s">
         <v>395</v>
       </c>
-      <c r="L58" s="55">
+      <c r="L58" s="48">
         <f>C58*K58</f>
         <v>2.66</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="49">
-        <f>ROW(B59) - ROW($B$9)</f>
+    <row r="59" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="12"/>
+      <c r="B59" s="42">
+        <f t="shared" si="17"/>
         <v>50</v>
       </c>
-      <c r="C59" s="51">
+      <c r="C59" s="44">
         <v>1</v>
       </c>
-      <c r="D59" s="68" t="s">
+      <c r="D59" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="E59" s="68" t="s">
+      <c r="E59" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="F59" s="68" t="s">
+      <c r="F59" s="59" t="s">
         <v>208</v>
       </c>
-      <c r="G59" s="68" t="s">
+      <c r="G59" s="59" t="s">
         <v>237</v>
       </c>
-      <c r="H59" s="68" t="s">
+      <c r="H59" s="59" t="s">
         <v>292</v>
       </c>
-      <c r="I59" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J59" s="68" t="s">
+      <c r="I59" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J59" s="59" t="s">
         <v>354</v>
       </c>
-      <c r="K59" s="71" t="s">
+      <c r="K59" s="62" t="s">
         <v>379</v>
       </c>
-      <c r="L59" s="57">
-        <f t="shared" ref="L59" si="24">C59*K59</f>
+      <c r="L59" s="50">
+        <f t="shared" ref="L59" si="26">C59*K59</f>
         <v>0.48</v>
       </c>
     </row>
     <row r="60" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="14"/>
-      <c r="B60" s="48">
-        <f>ROW(B60) - ROW($B$9)</f>
+      <c r="A60" s="12"/>
+      <c r="B60" s="41">
+        <f t="shared" si="17"/>
         <v>51</v>
       </c>
-      <c r="C60" s="50">
+      <c r="C60" s="43">
         <v>1</v>
       </c>
-      <c r="D60" s="67" t="s">
+      <c r="D60" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="E60" s="67" t="s">
+      <c r="E60" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="F60" s="69" t="s">
+      <c r="F60" s="60" t="s">
         <v>209</v>
       </c>
-      <c r="G60" s="69" t="s">
+      <c r="G60" s="60" t="s">
         <v>233</v>
       </c>
-      <c r="H60" s="69" t="s">
+      <c r="H60" s="60" t="s">
         <v>293</v>
       </c>
-      <c r="I60" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J60" s="69" t="s">
+      <c r="I60" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J60" s="60" t="s">
         <v>355</v>
       </c>
-      <c r="K60" s="70" t="s">
+      <c r="K60" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="L60" s="55">
+      <c r="L60" s="48">
         <f>C60*K60</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="14"/>
-      <c r="B61" s="49">
-        <f>ROW(B61) - ROW($B$9)</f>
+    <row r="61" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A61" s="12"/>
+      <c r="B61" s="42">
+        <f t="shared" si="17"/>
         <v>52</v>
       </c>
-      <c r="C61" s="51">
+      <c r="C61" s="44">
         <v>8</v>
       </c>
-      <c r="D61" s="68" t="s">
+      <c r="D61" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="E61" s="68" t="s">
+      <c r="E61" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="F61" s="68" t="s">
+      <c r="F61" s="59" t="s">
         <v>210</v>
       </c>
-      <c r="G61" s="68" t="s">
+      <c r="G61" s="59" t="s">
         <v>238</v>
       </c>
-      <c r="H61" s="68" t="s">
+      <c r="H61" s="59" t="s">
         <v>294</v>
       </c>
-      <c r="I61" s="68" t="s">
+      <c r="I61" s="59" t="s">
         <v>304</v>
       </c>
-      <c r="J61" s="68" t="s">
+      <c r="J61" s="59" t="s">
         <v>356</v>
       </c>
-      <c r="K61" s="71" t="s">
+      <c r="K61" s="62" t="s">
         <v>366</v>
       </c>
-      <c r="L61" s="57">
-        <f t="shared" ref="L61" si="25">C61*K61</f>
+      <c r="L61" s="50">
+        <f t="shared" ref="L61" si="27">C61*K61</f>
         <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
-      <c r="B62" s="48">
-        <f>ROW(B62) - ROW($B$9)</f>
+      <c r="A62" s="12"/>
+      <c r="B62" s="41">
+        <f t="shared" si="17"/>
         <v>53</v>
       </c>
-      <c r="C62" s="50">
+      <c r="C62" s="43">
         <v>1</v>
       </c>
-      <c r="D62" s="67" t="s">
+      <c r="D62" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="E62" s="67" t="s">
+      <c r="E62" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="F62" s="69" t="s">
+      <c r="F62" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="G62" s="69" t="s">
+      <c r="G62" s="60" t="s">
         <v>239</v>
       </c>
-      <c r="H62" s="69" t="s">
+      <c r="H62" s="60" t="s">
         <v>295</v>
       </c>
-      <c r="I62" s="69" t="s">
+      <c r="I62" s="60" t="s">
         <v>304</v>
       </c>
-      <c r="J62" s="69" t="s">
+      <c r="J62" s="60" t="s">
         <v>357</v>
       </c>
-      <c r="K62" s="70" t="s">
+      <c r="K62" s="61" t="s">
         <v>396</v>
       </c>
-      <c r="L62" s="55">
+      <c r="L62" s="48">
         <f>C62*K62</f>
         <v>0.97</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="49">
-        <f>ROW(B63) - ROW($B$9)</f>
+    <row r="63" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="12"/>
+      <c r="B63" s="42">
+        <f t="shared" si="17"/>
         <v>54</v>
       </c>
-      <c r="C63" s="51">
+      <c r="C63" s="44">
         <v>5</v>
       </c>
-      <c r="D63" s="68" t="s">
+      <c r="D63" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="E63" s="68" t="s">
+      <c r="E63" s="59" t="s">
         <v>152</v>
       </c>
-      <c r="F63" s="68" t="s">
+      <c r="F63" s="59" t="s">
         <v>212</v>
       </c>
-      <c r="G63" s="68" t="s">
+      <c r="G63" s="59" t="s">
         <v>239</v>
       </c>
-      <c r="H63" s="68" t="s">
+      <c r="H63" s="59" t="s">
         <v>296</v>
       </c>
-      <c r="I63" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J63" s="68" t="s">
+      <c r="I63" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J63" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="K63" s="71" t="s">
+      <c r="K63" s="62" t="s">
         <v>397</v>
       </c>
-      <c r="L63" s="57">
-        <f t="shared" ref="L63" si="26">C63*K63</f>
+      <c r="L63" s="50">
+        <f t="shared" ref="L63" si="28">C63*K63</f>
         <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="64" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="48">
-        <f>ROW(B64) - ROW($B$9)</f>
+      <c r="A64" s="12"/>
+      <c r="B64" s="41">
+        <f t="shared" si="17"/>
         <v>55</v>
       </c>
-      <c r="C64" s="50">
+      <c r="C64" s="43">
         <v>2</v>
       </c>
-      <c r="D64" s="67" t="s">
+      <c r="D64" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="E64" s="67" t="s">
+      <c r="E64" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="F64" s="69" t="s">
+      <c r="F64" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="G64" s="69" t="s">
+      <c r="G64" s="60" t="s">
         <v>240</v>
       </c>
-      <c r="H64" s="69" t="s">
+      <c r="H64" s="60" t="s">
         <v>297</v>
       </c>
-      <c r="I64" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J64" s="69" t="s">
+      <c r="I64" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J64" s="60" t="s">
         <v>359</v>
       </c>
-      <c r="K64" s="70" t="s">
+      <c r="K64" s="61" t="s">
         <v>398</v>
       </c>
-      <c r="L64" s="55">
+      <c r="L64" s="48">
         <f>C64*K64</f>
         <v>3.64</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="49">
-        <f>ROW(B65) - ROW($B$9)</f>
+    <row r="65" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="12"/>
+      <c r="B65" s="42">
+        <f t="shared" si="17"/>
         <v>56</v>
       </c>
-      <c r="C65" s="51">
+      <c r="C65" s="44">
         <v>1</v>
       </c>
-      <c r="D65" s="68" t="s">
+      <c r="D65" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="E65" s="68" t="s">
+      <c r="E65" s="59" t="s">
         <v>154</v>
       </c>
-      <c r="F65" s="68" t="s">
+      <c r="F65" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="G65" s="68" t="s">
+      <c r="G65" s="59" t="s">
         <v>239</v>
       </c>
-      <c r="H65" s="68" t="s">
+      <c r="H65" s="59" t="s">
         <v>298</v>
       </c>
-      <c r="I65" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J65" s="68" t="s">
+      <c r="I65" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J65" s="59" t="s">
         <v>360</v>
       </c>
-      <c r="K65" s="71" t="s">
+      <c r="K65" s="62" t="s">
         <v>399</v>
       </c>
-      <c r="L65" s="57">
-        <f t="shared" ref="L65" si="27">C65*K65</f>
+      <c r="L65" s="50">
+        <f t="shared" ref="L65" si="29">C65*K65</f>
         <v>2.33</v>
       </c>
     </row>
     <row r="66" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="48">
-        <f>ROW(B66) - ROW($B$9)</f>
+      <c r="A66" s="12"/>
+      <c r="B66" s="41">
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
-      <c r="C66" s="50">
+      <c r="C66" s="43">
         <v>1</v>
       </c>
-      <c r="D66" s="67" t="s">
+      <c r="D66" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="E66" s="67" t="s">
+      <c r="E66" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="F66" s="69" t="s">
+      <c r="F66" s="60" t="s">
         <v>215</v>
       </c>
-      <c r="G66" s="69" t="s">
+      <c r="G66" s="60" t="s">
         <v>240</v>
       </c>
-      <c r="H66" s="69" t="s">
+      <c r="H66" s="60" t="s">
         <v>299</v>
       </c>
-      <c r="I66" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J66" s="69" t="s">
+      <c r="I66" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J66" s="60" t="s">
         <v>361</v>
       </c>
-      <c r="K66" s="70" t="s">
+      <c r="K66" s="61" t="s">
         <v>400</v>
       </c>
-      <c r="L66" s="55">
+      <c r="L66" s="48">
         <f>C66*K66</f>
         <v>0.39</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="14"/>
-      <c r="B67" s="49">
-        <f>ROW(B67) - ROW($B$9)</f>
+    <row r="67" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="12"/>
+      <c r="B67" s="42">
+        <f t="shared" si="17"/>
         <v>58</v>
       </c>
-      <c r="C67" s="51">
+      <c r="C67" s="44">
         <v>2</v>
       </c>
-      <c r="D67" s="68" t="s">
+      <c r="D67" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="E67" s="68" t="s">
+      <c r="E67" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="F67" s="68" t="s">
+      <c r="F67" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="G67" s="68" t="s">
+      <c r="G67" s="59" t="s">
         <v>239</v>
       </c>
-      <c r="H67" s="68" t="s">
+      <c r="H67" s="59" t="s">
         <v>300</v>
       </c>
-      <c r="I67" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="J67" s="68" t="s">
+      <c r="I67" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="J67" s="59" t="s">
         <v>362</v>
       </c>
-      <c r="K67" s="71" t="s">
+      <c r="K67" s="62" t="s">
         <v>389</v>
       </c>
-      <c r="L67" s="57">
-        <f t="shared" ref="L67" si="28">C67*K67</f>
+      <c r="L67" s="50">
+        <f t="shared" ref="L67" si="30">C67*K67</f>
         <v>0.9</v>
       </c>
     </row>
     <row r="68" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="48">
-        <f>ROW(B68) - ROW($B$9)</f>
+      <c r="A68" s="12"/>
+      <c r="B68" s="41">
+        <f t="shared" si="17"/>
         <v>59</v>
       </c>
-      <c r="C68" s="50">
+      <c r="C68" s="43">
         <v>1</v>
       </c>
-      <c r="D68" s="67" t="s">
+      <c r="D68" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="E68" s="67" t="s">
+      <c r="E68" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="F68" s="69" t="s">
+      <c r="F68" s="60" t="s">
         <v>217</v>
       </c>
-      <c r="G68" s="69" t="s">
+      <c r="G68" s="60" t="s">
         <v>241</v>
       </c>
-      <c r="H68" s="69" t="s">
+      <c r="H68" s="60" t="s">
         <v>301</v>
       </c>
-      <c r="I68" s="69" t="s">
-        <v>303</v>
-      </c>
-      <c r="J68" s="69" t="s">
+      <c r="I68" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="J68" s="60" t="s">
         <v>363</v>
       </c>
-      <c r="K68" s="70" t="s">
+      <c r="K68" s="61" t="s">
         <v>401</v>
       </c>
-      <c r="L68" s="55">
+      <c r="L68" s="48">
         <f>C68*K68</f>
         <v>57.5</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="58" t="s">
+      <c r="A69" s="12"/>
+      <c r="B69" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C69" s="59"/>
-      <c r="D69" s="59"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="46"/>
+      <c r="C69" s="67"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="40"/>
+      <c r="F69" s="75"/>
       <c r="G69" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J69" s="53" t="s">
+      <c r="J69" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="K69" s="54"/>
-      <c r="L69" s="56">
+      <c r="K69" s="47"/>
+      <c r="L69" s="49">
         <f>SUM(L10:L68)</f>
         <v>268.95999999999992</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
+      <c r="A70" s="12"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
       <c r="E70" s="9"/>
-      <c r="F70" s="11"/>
+      <c r="F70" s="76"/>
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
-      <c r="L70" s="19"/>
+      <c r="L70" s="16"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
+      <c r="A71" s="12"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
       <c r="E71" s="10"/>
-      <c r="F71" s="12"/>
+      <c r="F71" s="77"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
-      <c r="L71" s="20"/>
+      <c r="L71" s="17"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
+      <c r="A72" s="12"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
       <c r="E72" s="10"/>
-      <c r="F72" s="12"/>
+      <c r="F72" s="77"/>
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
       <c r="I72" s="9"/>
@@ -4978,44 +5007,44 @@
         <v>22</v>
       </c>
       <c r="K72" s="9"/>
-      <c r="L72" s="20"/>
+      <c r="L72" s="17"/>
     </row>
     <row r="73" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="44"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
-      <c r="K73" s="16"/>
-      <c r="L73" s="21"/>
+      <c r="A73" s="12"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="78"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="18"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
+      <c r="F75" s="79"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+      <c r="F76" s="79"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
+      <c r="F77" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B69:D69"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.46" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="60" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="54" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;BAltium Limited Confidential&amp;B&amp;C&amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
@@ -5037,130 +5066,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="63" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="64" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="65" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="64" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="65" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="64" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="65" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="64" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="65" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="64" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="65" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="64" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="65" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="64" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="65" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="64" t="s">
         <v>410</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Replaced D6 from 1A to 2A diode. Added pi filter on output of power supply. Added 2x single pole filter on the use of 1.65V reference. Minor changes to layout and misc
</commit_message>
<xml_diff>
--- a/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
+++ b/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{797029B6-1F2C-432E-A167-2997CF08EEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{920BB682-B9A5-42C2-A96F-896E15CD7193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="433">
   <si>
     <t>Project Full Path</t>
   </si>
@@ -127,10 +127,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>4/15/2025</t>
-  </si>
-  <si>
-    <t>6:24:11 AM</t>
+    <t>5/11/2025</t>
+  </si>
+  <si>
+    <t>8:44:53 AM</t>
   </si>
   <si>
     <t>Arbitrary Power Booster</t>
@@ -139,7 +139,7 @@
     <t>IMR-005-SCH</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
   <si>
     <t>Hab S Collector</t>
@@ -178,6 +178,18 @@
     <t>DIODE_SCHOTTKY_1N5819HW-7-F</t>
   </si>
   <si>
+    <t>DIODE_SCHOTTKY_B240S1F-7</t>
+  </si>
+  <si>
+    <t>FAN_AFB0405LA-A</t>
+  </si>
+  <si>
+    <t>FERRITE_2508053017Y3</t>
+  </si>
+  <si>
+    <t>HEATSINK_CS9464020BP</t>
+  </si>
+  <si>
     <t>CONN_PANOMA_73099-2</t>
   </si>
   <si>
@@ -196,6 +208,15 @@
     <t>INDUCTOR_SRN4018TA-6R8M</t>
   </si>
   <si>
+    <t>LED_RED_LTST-C170EKT</t>
+  </si>
+  <si>
+    <t>MECHANICAL_SCREW_M3X6_PAN_HEAD</t>
+  </si>
+  <si>
+    <t>MECHANICAL_STANDOFF_M3X20</t>
+  </si>
+  <si>
     <t>MOSFET_PCH_DMP6050SPS-13</t>
   </si>
   <si>
@@ -205,22 +226,7 @@
     <t>MOSFET_NCH_DMNH6042SPDQ-13</t>
   </si>
   <si>
-    <t>BJT_PNP_2SAR582D3FRATL</t>
-  </si>
-  <si>
-    <t>BJT_NPN_MMBT4401LT1G</t>
-  </si>
-  <si>
-    <t>BJT_PNP_DJT4030P-13</t>
-  </si>
-  <si>
-    <t>BJT_NPN_DJT4031N-13</t>
-  </si>
-  <si>
-    <t>BJT_PNP_MMBT4403LT1G</t>
-  </si>
-  <si>
-    <t>BJT_NPN_2SCR582D3FRATL</t>
+    <t>MOSFET_NCH_DMN3023L-7</t>
   </si>
   <si>
     <t>RES_SMD_0_2512_1W_1%</t>
@@ -250,13 +256,7 @@
     <t>RES_SMD_13.7K_0805_1/8W_1%</t>
   </si>
   <si>
-    <t>RES_SMD_240_2512_3W_5%</t>
-  </si>
-  <si>
-    <t>RES_SMD_270_2512_3W_5%</t>
-  </si>
-  <si>
-    <t>RES_SMD_10_0805_1/8W_1%</t>
+    <t>RES_SMD_300_0805_1/8W_1%</t>
   </si>
   <si>
     <t>RES_SMD_1M_0805_1/4W_1%</t>
@@ -265,9 +265,6 @@
     <t>RES_SMD_100_0805_3.5W_1%</t>
   </si>
   <si>
-    <t>RES_SMD_0.2_1206_1/4W_1%</t>
-  </si>
-  <si>
     <t>RES_SMD_1.5K_0805_1/8W_1%</t>
   </si>
   <si>
@@ -280,18 +277,18 @@
     <t>RES_SMD_0.0065_2512_2W_1%</t>
   </si>
   <si>
-    <t>RES_SMD_200_0805_1/8W_1%</t>
+    <t>RES_SMD_3.0K_0805_1/8W_1%</t>
   </si>
   <si>
     <t>RES_SMD_4.99K_0805_1/8W_1%</t>
   </si>
   <si>
-    <t>RES_SMD_3.0K_0805_1/8W_1%</t>
-  </si>
-  <si>
     <t>RES_SMD_2.49K_0805_1/8W_1%</t>
   </si>
   <si>
+    <t>RES_SMD_100_0805_1/8W_1%</t>
+  </si>
+  <si>
     <t>RELAY_AZ733-2AE-5DE</t>
   </si>
   <si>
@@ -322,6 +319,9 @@
     <t>IC_MCP45HV51-104E/ST</t>
   </si>
   <si>
+    <t>IC_SN74LVC1G14DCKR</t>
+  </si>
+  <si>
     <t>OPAMP_LMP2011MFX/NOPB</t>
   </si>
   <si>
@@ -334,6 +334,9 @@
     <t>MODULE_STM32F746G-DISCO</t>
   </si>
   <si>
+    <t>OPAMP_OPA549S</t>
+  </si>
+  <si>
     <t>OPAMP_TLV9302IDR</t>
   </si>
   <si>
@@ -367,6 +370,18 @@
     <t>DIODE SCHOTTKY 40V 1A SOD123</t>
   </si>
   <si>
+    <t>DIODE SCHOTTKY 40V 2A SOD123F</t>
+  </si>
+  <si>
+    <t>FAN AXIAL 40X10MM BALL 5VDC WIRE</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 300 OHM 0805 1LN</t>
+  </si>
+  <si>
+    <t>Heat Sink Aluminum Top Mount</t>
+  </si>
+  <si>
     <t>CONN 4mm Banana Socket Right Angle PCB RED</t>
   </si>
   <si>
@@ -385,6 +400,15 @@
     <t>FIXED IND 6.8UH 1.7A 98 MOHM SMD</t>
   </si>
   <si>
+    <t>LED RED CLEAR SMD</t>
+  </si>
+  <si>
+    <t>SCREW M3X6 PAN HEAD SS</t>
+  </si>
+  <si>
+    <t>HEX STANDOFF M3 BRASS 20MM</t>
+  </si>
+  <si>
     <t>MOSFET P-CH 60V 5.7A PWRDI5060-8</t>
   </si>
   <si>
@@ -394,22 +418,7 @@
     <t>MOSFET NCH 60V 5.7A POWERDI</t>
   </si>
   <si>
-    <t>TRANS PNP 30V 5.7A TO-252</t>
-  </si>
-  <si>
-    <t>TRANS NPN 40V 0.6A SOT23-3</t>
-  </si>
-  <si>
-    <t>TRANS PNP 40V 3A SOT223</t>
-  </si>
-  <si>
-    <t>TRANS NPN 40V 3A SOT223</t>
-  </si>
-  <si>
-    <t>TRANS PNP 40V 0.6A SOT23-3</t>
-  </si>
-  <si>
-    <t>TRANS NPN 30V 10A TO-252</t>
+    <t>MOSFET N-CH 30V 6.2A SOT23-3</t>
   </si>
   <si>
     <t>RES SMD 0 OHM 1% 1W 2512</t>
@@ -439,13 +448,7 @@
     <t>RES SMD 13.7K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>RES 240 OHM 5% 3W 2512</t>
-  </si>
-  <si>
-    <t>RES 270 OHM 5% 1W 2512</t>
-  </si>
-  <si>
-    <t>RES SMD 10 OHM 1% 1/8W 0805</t>
+    <t>RES SMD 300 OHM 1% 1/8W 0805</t>
   </si>
   <si>
     <t>RES SMD 1K OHM 1% 1/4W 0805</t>
@@ -454,9 +457,6 @@
     <t>RES SMD 100 OHM 1% 3.5W 2512</t>
   </si>
   <si>
-    <t>RES SMD 0.2 OHM 1% 1/4W 1206</t>
-  </si>
-  <si>
     <t>RES SMD 1.5K OHM 1% 1/8W 0805</t>
   </si>
   <si>
@@ -469,18 +469,18 @@
     <t>RES SMD 0.0065 OHM 1% 2W 2512</t>
   </si>
   <si>
-    <t>RES SMD 200 OHM 1% 1/8W 0805</t>
+    <t>RES SMD 3.0K OHM 1% 1/8W 0805</t>
   </si>
   <si>
     <t>RES SMD 4.99K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>RES SMD 3.0K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
     <t>RES SMD 2.49K OHM 1% 1/8W 0805</t>
   </si>
   <si>
+    <t>RES SMD 100 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
     <t>RELAY GEN PURPOSE SPDT 10A 5V</t>
   </si>
   <si>
@@ -505,6 +505,9 @@
     <t>IC DGT POT 100KOHM 256TP 14TSSOP</t>
   </si>
   <si>
+    <t>IC INVERT SCHMITT 1CH 1IN SC70-5</t>
+  </si>
+  <si>
     <t>IC OPAMP GP 3MHZ .12uV CIRCUIT SOT23-5</t>
   </si>
   <si>
@@ -517,6 +520,9 @@
     <t>DISCOVERY STM32 F7 EVAL BRD</t>
   </si>
   <si>
+    <t>IC OPAMP POWER 1 CIRC 11PWRPACK</t>
+  </si>
+  <si>
     <t>IC OPAMP GP 2 CIRCUIT 8SOIC</t>
   </si>
   <si>
@@ -529,25 +535,37 @@
     <t>C4, C12, C16</t>
   </si>
   <si>
-    <t>C5, C6, C7, C8, C13, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43, C44</t>
+    <t>C5, C6, C7, C8, C13, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46</t>
   </si>
   <si>
     <t>C14</t>
   </si>
   <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>C30, C31, C32</t>
+    <t>C15, C48</t>
+  </si>
+  <si>
+    <t>C30, C31, C32, C47</t>
   </si>
   <si>
     <t>D1, D5</t>
   </si>
   <si>
-    <t>D2, D3, D7, D9, D10, D11, D12, D13, D14, D15, D16</t>
-  </si>
-  <si>
-    <t>D4, D6, D8</t>
+    <t>D2, D3, D7, D9, D10, D11, D12, D13, D14, D15, D16, D17, D18, D19, D20, D21, D22</t>
+  </si>
+  <si>
+    <t>D4, D8</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>FAN1, FAN2</t>
+  </si>
+  <si>
+    <t>FB1</t>
+  </si>
+  <si>
+    <t>HS1, HS2</t>
   </si>
   <si>
     <t>J1, J4, J6, J10</t>
@@ -562,43 +580,37 @@
     <t>J8</t>
   </si>
   <si>
-    <t>JP1, JP2, JP3, JP4, JP5, JP6, JP7, JP8, JP9, JP10, JP11, JP12, JP13</t>
+    <t>JP1, JP2, JP3, JP4</t>
   </si>
   <si>
     <t>L1</t>
   </si>
   <si>
+    <t>LED1, LED2</t>
+  </si>
+  <si>
+    <t>MECH1, MECH2, MECH3, MECH4, MECH9, MECH10, MECH11, MECH12</t>
+  </si>
+  <si>
+    <t>MECH5, MECH6, MECH7, MECH8</t>
+  </si>
+  <si>
     <t>Q1, Q2</t>
   </si>
   <si>
-    <t>Q3, Q8, Q18, Q28, Q38, Q45, Q46</t>
+    <t>Q3, Q7, Q8, Q9, Q10, Q11, Q12</t>
   </si>
   <si>
     <t>Q4</t>
   </si>
   <si>
-    <t>Q5, Q12, Q13, Q14, Q25, Q32, Q33, Q34</t>
-  </si>
-  <si>
-    <t>Q6, Q15, Q16, Q17, Q26, Q35, Q36, Q37</t>
-  </si>
-  <si>
-    <t>Q7, Q27</t>
-  </si>
-  <si>
-    <t>Q9, Q29</t>
-  </si>
-  <si>
-    <t>Q10, Q19, Q20, Q21, Q30, Q39, Q40, Q41</t>
-  </si>
-  <si>
-    <t>Q11, Q22, Q23, Q24, Q31, Q42, Q43, Q44</t>
+    <t>Q5, Q6</t>
   </si>
   <si>
     <t>R1, R6</t>
   </si>
   <si>
-    <t>R2, R3, R7, R8, R11, R27, R30, R31, R32, R45, R51, R52, R53, R63, R66, R67, R75, R77, R79, R81, R82, R84, R85, R86, R89, R90, R93, R94</t>
+    <t>R2, R3, R7, R8, R11, R25, R27, R30, R31, R32, R37, R38, R42, R43, R45, R46, R47, R51, R52, R53, R54, R61, R62, R63, R64, R65, R66, R67, R69, R72</t>
   </si>
   <si>
     <t>R4, R13</t>
@@ -610,7 +622,7 @@
     <t>R9</t>
   </si>
   <si>
-    <t>R10, R50</t>
+    <t>R10, R18, R19, R24, R26, R28, R36, R50</t>
   </si>
   <si>
     <t>R12, R16</t>
@@ -622,13 +634,7 @@
     <t>R17</t>
   </si>
   <si>
-    <t>R18, R28, R54, R64</t>
-  </si>
-  <si>
-    <t>R19, R29, R55, R65</t>
-  </si>
-  <si>
-    <t>R20, R26, R56, R62</t>
+    <t>R20, R29</t>
   </si>
   <si>
     <t>R21, R57</t>
@@ -637,13 +643,10 @@
     <t>R22, R23, R58, R59</t>
   </si>
   <si>
-    <t>R24, R25, R36, R37, R38, R40, R41, R42, R60, R61, R68, R69, R70, R72, R73, R74</t>
-  </si>
-  <si>
     <t>R33</t>
   </si>
   <si>
-    <t>R34, R80, R83</t>
+    <t>R34, R60, R70</t>
   </si>
   <si>
     <t>R35</t>
@@ -652,16 +655,16 @@
     <t>R39, R71</t>
   </si>
   <si>
-    <t>R43, R44, R46, R47</t>
-  </si>
-  <si>
-    <t>R48, R78, R87, R92</t>
-  </si>
-  <si>
-    <t>R49, R91</t>
-  </si>
-  <si>
-    <t>R76, R88</t>
+    <t>R40, R49</t>
+  </si>
+  <si>
+    <t>R41, R48, R55, R68</t>
+  </si>
+  <si>
+    <t>R44, R56</t>
+  </si>
+  <si>
+    <t>R73, R74</t>
   </si>
   <si>
     <t>REL1</t>
@@ -682,18 +685,21 @@
     <t>SW2</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP11</t>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
-    <t>U2, U3, U5, U10, U12, U16, U17</t>
+    <t>U2, U3, U10</t>
   </si>
   <si>
     <t>U4, U11</t>
   </si>
   <si>
+    <t>U5, U16</t>
+  </si>
+  <si>
     <t>U6</t>
   </si>
   <si>
@@ -706,6 +712,9 @@
     <t>U9</t>
   </si>
   <si>
+    <t>U12, U17</t>
+  </si>
+  <si>
     <t>U14, U15</t>
   </si>
   <si>
@@ -727,6 +736,15 @@
     <t>Diodes Inc</t>
   </si>
   <si>
+    <t>Delta Electronicis</t>
+  </si>
+  <si>
+    <t>Fair-Rite</t>
+  </si>
+  <si>
+    <t>Cooling Source</t>
+  </si>
+  <si>
     <t>Pomona</t>
   </si>
   <si>
@@ -739,10 +757,10 @@
     <t>Bourns Inc.</t>
   </si>
   <si>
-    <t>Rohm Semiconductor</t>
-  </si>
-  <si>
-    <t>On Semiconductor</t>
+    <t>APM Hexseal</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
   </si>
   <si>
     <t>Yageo</t>
@@ -811,6 +829,18 @@
     <t>1N5819HW-7-F</t>
   </si>
   <si>
+    <t>B240S1F-7</t>
+  </si>
+  <si>
+    <t>AFB0405LA-A</t>
+  </si>
+  <si>
+    <t>2508053017Y3</t>
+  </si>
+  <si>
+    <t>CS9464020BP</t>
+  </si>
+  <si>
     <t>73099-2</t>
   </si>
   <si>
@@ -829,6 +859,15 @@
     <t>SRN4018TA-6R8M</t>
   </si>
   <si>
+    <t>LTST-C170EKT</t>
+  </si>
+  <si>
+    <t>RM3X6MM 2701</t>
+  </si>
+  <si>
+    <t>24407</t>
+  </si>
+  <si>
     <t>DMP6050SPS-13</t>
   </si>
   <si>
@@ -838,22 +877,7 @@
     <t>DMNH6042SPDQ-13</t>
   </si>
   <si>
-    <t>2SAR582D3FRATL</t>
-  </si>
-  <si>
-    <t>MMBT4401LT1G</t>
-  </si>
-  <si>
-    <t>DJT4030P-13</t>
-  </si>
-  <si>
-    <t>DJT4031N-13</t>
-  </si>
-  <si>
-    <t>MMBT4403LT1G</t>
-  </si>
-  <si>
-    <t>2SCR582D3FRATL</t>
+    <t>DMN3023L-7</t>
   </si>
   <si>
     <t>RC2512JK-070RL</t>
@@ -883,13 +907,7 @@
     <t>RC0805FR-0713K7L</t>
   </si>
   <si>
-    <t>RC2512JK-07240RL</t>
-  </si>
-  <si>
-    <t>RC2512JK-07270RL</t>
-  </si>
-  <si>
-    <t>RC0805FR-1310RL</t>
+    <t>RC0805FR-07300RL</t>
   </si>
   <si>
     <t>RC0805FR-7W1ML</t>
@@ -898,9 +916,6 @@
     <t>ALN2512F100RE-1</t>
   </si>
   <si>
-    <t>RL1206FR-070R2L</t>
-  </si>
-  <si>
     <t>RC0805FR-071K5L</t>
   </si>
   <si>
@@ -913,18 +928,18 @@
     <t>WSL25126L500FEA18</t>
   </si>
   <si>
-    <t>RC0805FR-07200RL</t>
+    <t>RC0805FR-133KL</t>
   </si>
   <si>
     <t>RC0805FR-134K99L</t>
   </si>
   <si>
-    <t>RC0805FR-133KL</t>
-  </si>
-  <si>
     <t>RC0805FR-132K49L</t>
   </si>
   <si>
+    <t>RC0805FR-07100RL</t>
+  </si>
+  <si>
     <t>AZ733-2AE-5DE</t>
   </si>
   <si>
@@ -955,6 +970,9 @@
     <t>MCP45HV51-104E/ST</t>
   </si>
   <si>
+    <t>SN74LVC1G14DCKR</t>
+  </si>
+  <si>
     <t>LMP2011MFX/NOPB</t>
   </si>
   <si>
@@ -967,6 +985,9 @@
     <t>STM32F746G-DISCO</t>
   </si>
   <si>
+    <t>OPA549S</t>
+  </si>
+  <si>
     <t>TLV9302IDR</t>
   </si>
   <si>
@@ -1009,6 +1030,18 @@
     <t>1N5819HW-FDICT-ND</t>
   </si>
   <si>
+    <t>B240S1F-7DICT-ND</t>
+  </si>
+  <si>
+    <t>603-2014-ND</t>
+  </si>
+  <si>
+    <t>1934-1474-1-ND</t>
+  </si>
+  <si>
+    <t>4165-CS9464020BP-ND</t>
+  </si>
+  <si>
     <t>501-73099-2-ND</t>
   </si>
   <si>
@@ -1027,6 +1060,15 @@
     <t>SRN4018TA-6R8MCT-ND</t>
   </si>
   <si>
+    <t>160-1178-1-ND</t>
+  </si>
+  <si>
+    <t>335-1156-ND</t>
+  </si>
+  <si>
+    <t>36-24407-ND</t>
+  </si>
+  <si>
     <t>DMP6050SPS-13DICT-ND</t>
   </si>
   <si>
@@ -1036,22 +1078,7 @@
     <t>DMNH6042SPDQ-13DICT-ND</t>
   </si>
   <si>
-    <t>846-2SAR582D3FRATLCT-ND</t>
-  </si>
-  <si>
-    <t>MMBT4401LT1GOSCT-ND</t>
-  </si>
-  <si>
-    <t>31-DJT4030P-13CT-ND</t>
-  </si>
-  <si>
-    <t>DJT4031NDICT-ND</t>
-  </si>
-  <si>
-    <t>MMBT4403LT1GOSCT-ND</t>
-  </si>
-  <si>
-    <t>846-2SCR582D3FRATLCT-ND</t>
+    <t>DMN3023L-7DICT-ND</t>
   </si>
   <si>
     <t>YAG1232CT-ND</t>
@@ -1081,13 +1108,7 @@
     <t>311-13.7KCRCT-ND</t>
   </si>
   <si>
-    <t>13-RC2512JK-07240RLCT-ND</t>
-  </si>
-  <si>
-    <t>13-RC2512JK-07270RLCT-ND</t>
-  </si>
-  <si>
-    <t>13-RC0805FR-1310RLCT-ND</t>
+    <t>311-300CRCT-ND</t>
   </si>
   <si>
     <t>13-RC0805FR-7W1MLCT-ND</t>
@@ -1096,9 +1117,6 @@
     <t>273-ALN2512F100RE-1CT-ND</t>
   </si>
   <si>
-    <t>311-0.2LWCT-ND</t>
-  </si>
-  <si>
     <t>311-1.50KCRCT-ND</t>
   </si>
   <si>
@@ -1111,18 +1129,18 @@
     <t>541-WSL25126L500FEA18CT-ND</t>
   </si>
   <si>
-    <t>311-200CRCT-ND</t>
+    <t>13-RC0805FR-133KLCT-ND</t>
   </si>
   <si>
     <t>13-RC0805FR-134K99LCT-ND</t>
   </si>
   <si>
-    <t>13-RC0805FR-133KLCT-ND</t>
-  </si>
-  <si>
     <t>13-RC0805FR-132K49LCT-ND</t>
   </si>
   <si>
+    <t>311-100CRCT-ND</t>
+  </si>
+  <si>
     <t>3385-AZ733-2AE-5DE-nd</t>
   </si>
   <si>
@@ -1153,6 +1171,9 @@
     <t>MCP45HV51-104E/ST-ND</t>
   </si>
   <si>
+    <t>296-11608-1-ND</t>
+  </si>
+  <si>
     <t>LMP2011MFX/NOPBCT-ND</t>
   </si>
   <si>
@@ -1165,6 +1186,9 @@
     <t>497-15680-5-ND</t>
   </si>
   <si>
+    <t>OPA549S-ND</t>
+  </si>
+  <si>
     <t>296-53513-1-ND</t>
   </si>
   <si>
@@ -1195,6 +1219,15 @@
     <t>.25</t>
   </si>
   <si>
+    <t>7.31</t>
+  </si>
+  <si>
+    <t>.10</t>
+  </si>
+  <si>
+    <t>3.41</t>
+  </si>
+  <si>
     <t>10.39</t>
   </si>
   <si>
@@ -1207,42 +1240,30 @@
     <t>.48</t>
   </si>
   <si>
+    <t>.58</t>
+  </si>
+  <si>
+    <t>1.36</t>
+  </si>
+  <si>
     <t>1.07</t>
   </si>
   <si>
     <t>.20</t>
   </si>
   <si>
-    <t>1.36</t>
-  </si>
-  <si>
-    <t>1.59</t>
+    <t>.2</t>
   </si>
   <si>
     <t>.13</t>
   </si>
   <si>
-    <t>.76</t>
+    <t>1.50</t>
   </si>
   <si>
     <t>1.76</t>
   </si>
   <si>
-    <t>.2</t>
-  </si>
-  <si>
-    <t>.10</t>
-  </si>
-  <si>
-    <t>.21</t>
-  </si>
-  <si>
-    <t>1.50</t>
-  </si>
-  <si>
-    <t>.27</t>
-  </si>
-  <si>
     <t>2.18</t>
   </si>
   <si>
@@ -1276,16 +1297,19 @@
     <t>57.50</t>
   </si>
   <si>
+    <t>26.94</t>
+  </si>
+  <si>
     <t>.66</t>
   </si>
   <si>
     <t>C:\IMR_Projects\IMR\Arb_Power_Booster\Hardware\Arb_Power_Booster\Arb_Power_Booster.PrjPcb</t>
   </si>
   <si>
-    <t>259</t>
-  </si>
-  <si>
-    <t>4/15/2025 6:24:11 AM</t>
+    <t>223</t>
+  </si>
+  <si>
+    <t>5/11/2025 8:44:53 AM</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -2506,7 +2530,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -2667,11 +2691,11 @@
       </c>
       <c r="E8" s="38">
         <f ca="1">TODAY()</f>
-        <v>45762</v>
+        <v>45788</v>
       </c>
       <c r="F8" s="39">
         <f ca="1">NOW()</f>
-        <v>45762.267278009262</v>
+        <v>45788.36558784722</v>
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>
@@ -2691,25 +2715,25 @@
         <v>40</v>
       </c>
       <c r="E9" s="66" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G9" s="66" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="H9" s="66" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="I9" s="66" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="J9" s="66" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="K9" s="66" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="L9" s="25" t="s">
         <v>29</v>
@@ -2728,25 +2752,25 @@
         <v>41</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F10" s="69" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G10" s="69" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="H10" s="69" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="I10" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J10" s="69" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="K10" s="70" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="L10" s="55">
         <f>C10*K10</f>
@@ -2766,28 +2790,28 @@
         <v>42</v>
       </c>
       <c r="E11" s="68" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F11" s="68" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G11" s="68" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H11" s="68" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="I11" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J11" s="68" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="K11" s="71" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="L11" s="57">
-        <f t="shared" ref="L11:L71" si="0">C11*K11</f>
+        <f t="shared" ref="L11:L72" si="0">C11*K11</f>
         <v>0.84000000000000008</v>
       </c>
     </row>
@@ -2798,35 +2822,35 @@
         <v>3</v>
       </c>
       <c r="C12" s="50">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" s="67" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F12" s="69" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G12" s="69" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="H12" s="69" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="I12" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J12" s="69" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="K12" s="70" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L12" s="55">
         <f>C12*K12</f>
-        <v>3</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2842,25 +2866,25 @@
         <v>44</v>
       </c>
       <c r="E13" s="68" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F13" s="68" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G13" s="68" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H13" s="68" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="I13" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J13" s="68" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="K13" s="71" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="L13" s="57">
         <f t="shared" ref="L13" si="1">C13*K13</f>
@@ -2874,35 +2898,35 @@
         <v>5</v>
       </c>
       <c r="C14" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="67" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F14" s="69" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G14" s="69" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H14" s="69" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="I14" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J14" s="69" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="K14" s="70" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="L14" s="55">
         <f>C14*K14</f>
-        <v>0.28000000000000003</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2912,35 +2936,35 @@
         <v>6</v>
       </c>
       <c r="C15" s="51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="68" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="68" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F15" s="68" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G15" s="68" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H15" s="68" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="I15" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J15" s="68" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="K15" s="71" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="L15" s="57">
         <f t="shared" ref="L15" si="2">C15*K15</f>
-        <v>17.04</v>
+        <v>22.72</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2956,25 +2980,25 @@
         <v>47</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F16" s="69" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G16" s="69" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="H16" s="69" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="I16" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J16" s="69" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="K16" s="70" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="L16" s="55">
         <f>C16*K16</f>
@@ -2988,35 +3012,35 @@
         <v>8</v>
       </c>
       <c r="C17" s="51">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D17" s="68" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="68" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F17" s="68" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G17" s="68" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="H17" s="68" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="I17" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J17" s="68" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="K17" s="71" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="L17" s="57">
         <f t="shared" ref="L17" si="3">C17*K17</f>
-        <v>1.76</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
@@ -3026,35 +3050,35 @@
         <v>9</v>
       </c>
       <c r="C18" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="67" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F18" s="69" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G18" s="69" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="H18" s="69" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="I18" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J18" s="69" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="K18" s="70" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="L18" s="55">
         <f>C18*K18</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3064,35 +3088,35 @@
         <v>10</v>
       </c>
       <c r="C19" s="51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D19" s="68" t="s">
         <v>50</v>
       </c>
       <c r="E19" s="68" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F19" s="68" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G19" s="68" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H19" s="68" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="I19" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J19" s="68" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="K19" s="71" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="L19" s="57">
         <f t="shared" ref="L19" si="4">C19*K19</f>
-        <v>41.56</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3102,35 +3126,35 @@
         <v>11</v>
       </c>
       <c r="C20" s="50">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D20" s="67" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="67" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F20" s="69" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G20" s="69" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="H20" s="69" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="I20" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J20" s="69" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="K20" s="70" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="L20" s="55">
         <f>C20*K20</f>
-        <v>41.56</v>
+        <v>14.62</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3140,35 +3164,35 @@
         <v>12</v>
       </c>
       <c r="C21" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E21" s="68" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F21" s="68" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G21" s="68" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="H21" s="68" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="I21" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J21" s="68" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="K21" s="71" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="L21" s="57">
         <f t="shared" ref="L21" si="5">C21*K21</f>
-        <v>2.8</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3178,35 +3202,35 @@
         <v>13</v>
       </c>
       <c r="C22" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="67" t="s">
         <v>53</v>
       </c>
       <c r="E22" s="67" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F22" s="69" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G22" s="69" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="H22" s="69" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="I22" s="69" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="J22" s="69" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="K22" s="70" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="L22" s="55">
         <f>C22*K22</f>
-        <v>7.0000000000000007E-2</v>
+        <v>6.82</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3216,35 +3240,35 @@
         <v>14</v>
       </c>
       <c r="C23" s="51">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D23" s="68" t="s">
         <v>54</v>
       </c>
       <c r="E23" s="68" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F23" s="68" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G23" s="68" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H23" s="68" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="I23" s="68" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="J23" s="68" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="K23" s="71" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="L23" s="57">
         <f t="shared" ref="L23" si="6">C23*K23</f>
-        <v>0.91000000000000014</v>
+        <v>41.56</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3254,35 +3278,35 @@
         <v>15</v>
       </c>
       <c r="C24" s="50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D24" s="67" t="s">
         <v>55</v>
       </c>
       <c r="E24" s="67" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F24" s="69" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G24" s="69" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="H24" s="69" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="I24" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J24" s="69" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="K24" s="70" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="L24" s="55">
         <f>C24*K24</f>
-        <v>0.48</v>
+        <v>41.56</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3298,29 +3322,29 @@
         <v>56</v>
       </c>
       <c r="E25" s="68" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F25" s="68" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G25" s="68" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="H25" s="68" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="I25" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J25" s="68" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="K25" s="71" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="L25" s="57">
         <f t="shared" ref="L25" si="7">C25*K25</f>
-        <v>2.14</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3330,35 +3354,35 @@
         <v>17</v>
       </c>
       <c r="C26" s="50">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D26" s="67" t="s">
         <v>57</v>
       </c>
       <c r="E26" s="67" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F26" s="69" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G26" s="69" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="H26" s="69" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="I26" s="69" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="J26" s="69" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="K26" s="70" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="L26" s="55">
         <f>C26*K26</f>
-        <v>1.4000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3368,73 +3392,73 @@
         <v>18</v>
       </c>
       <c r="C27" s="51">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D27" s="68" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F27" s="68" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G27" s="68" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="H27" s="68" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="I27" s="68" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="J27" s="68" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="K27" s="71" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="L27" s="57">
         <f t="shared" ref="L27" si="8">C27*K27</f>
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
       <c r="B28" s="48">
         <f>ROW(B28) - ROW($B$9)</f>
         <v>19</v>
       </c>
       <c r="C28" s="50">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D28" s="67" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="67" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F28" s="69" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G28" s="69" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="H28" s="69" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="I28" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J28" s="69" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="K28" s="70" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="L28" s="55">
         <f>C28*K28</f>
-        <v>12.72</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3444,73 +3468,73 @@
         <v>20</v>
       </c>
       <c r="C29" s="51">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D29" s="68" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="68" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F29" s="68" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G29" s="68" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H29" s="68" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="I29" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J29" s="68" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="K29" s="71" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="L29" s="57">
         <f t="shared" ref="L29" si="9">C29*K29</f>
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="3" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="48">
         <f>ROW(B30) - ROW($B$9)</f>
         <v>21</v>
       </c>
       <c r="C30" s="50">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D30" s="67" t="s">
         <v>61</v>
       </c>
       <c r="E30" s="67" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F30" s="69" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G30" s="69" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="H30" s="69" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="I30" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J30" s="69" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="K30" s="70" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="L30" s="55">
         <f>C30*K30</f>
-        <v>1.52</v>
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3520,73 +3544,73 @@
         <v>22</v>
       </c>
       <c r="C31" s="51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D31" s="68" t="s">
         <v>62</v>
       </c>
       <c r="E31" s="68" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F31" s="68" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G31" s="68" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H31" s="68" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="I31" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J31" s="68" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="K31" s="71" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="L31" s="57">
         <f t="shared" ref="L31" si="10">C31*K31</f>
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14"/>
       <c r="B32" s="48">
         <f>ROW(B32) - ROW($B$9)</f>
         <v>23</v>
       </c>
       <c r="C32" s="50">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D32" s="67" t="s">
         <v>63</v>
       </c>
       <c r="E32" s="67" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F32" s="69" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G32" s="69" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H32" s="69" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="I32" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J32" s="69" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="K32" s="70" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="L32" s="55">
         <f>C32*K32</f>
-        <v>1.04</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3596,73 +3620,73 @@
         <v>24</v>
       </c>
       <c r="C33" s="51">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E33" s="68" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F33" s="68" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G33" s="68" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H33" s="68" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="I33" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J33" s="68" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="K33" s="71" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="L33" s="57">
         <f t="shared" ref="L33" si="11">C33*K33</f>
-        <v>14.08</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A34" s="14"/>
       <c r="B34" s="48">
         <f>ROW(B34) - ROW($B$9)</f>
         <v>25</v>
       </c>
       <c r="C34" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="67" t="s">
         <v>65</v>
       </c>
       <c r="E34" s="67" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F34" s="69" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G34" s="69" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H34" s="69" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="I34" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J34" s="69" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="K34" s="70" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="L34" s="55">
         <f>C34*K34</f>
-        <v>0.4</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3672,35 +3696,35 @@
         <v>26</v>
       </c>
       <c r="C35" s="51">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D35" s="68" t="s">
         <v>66</v>
       </c>
       <c r="E35" s="68" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F35" s="68" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G35" s="68" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H35" s="68" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="I35" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J35" s="68" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="K35" s="71" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="L35" s="57">
         <f t="shared" ref="L35" si="12">C35*K35</f>
-        <v>2.8000000000000003</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3716,29 +3740,29 @@
         <v>67</v>
       </c>
       <c r="E36" s="67" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F36" s="69" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G36" s="69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H36" s="69" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="I36" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J36" s="69" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="K36" s="70" t="s">
-        <v>383</v>
+        <v>408</v>
       </c>
       <c r="L36" s="55">
         <f>C36*K36</f>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3748,35 +3772,35 @@
         <v>28</v>
       </c>
       <c r="C37" s="51">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D37" s="68" t="s">
         <v>68</v>
       </c>
       <c r="E37" s="68" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F37" s="68" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G37" s="68" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H37" s="68" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="I37" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J37" s="68" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="K37" s="71" t="s">
-        <v>383</v>
+        <v>398</v>
       </c>
       <c r="L37" s="57">
         <f t="shared" ref="L37" si="13">C37*K37</f>
-        <v>0.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3786,35 +3810,35 @@
         <v>29</v>
       </c>
       <c r="C38" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="67" t="s">
         <v>69</v>
       </c>
       <c r="E38" s="67" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F38" s="69" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G38" s="69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H38" s="69" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="I38" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J38" s="69" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="K38" s="70" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L38" s="55">
         <f>C38*K38</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3830,25 +3854,25 @@
         <v>70</v>
       </c>
       <c r="E39" s="68" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F39" s="68" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G39" s="68" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H39" s="68" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="I39" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J39" s="68" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="K39" s="71" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L39" s="57">
         <f t="shared" ref="L39" si="14">C39*K39</f>
@@ -3862,35 +3886,35 @@
         <v>31</v>
       </c>
       <c r="C40" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" s="67" t="s">
         <v>71</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F40" s="69" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G40" s="69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H40" s="69" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="I40" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J40" s="69" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K40" s="70" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L40" s="55">
         <f>C40*K40</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3900,35 +3924,35 @@
         <v>32</v>
       </c>
       <c r="C41" s="51">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D41" s="68" t="s">
         <v>72</v>
       </c>
       <c r="E41" s="68" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F41" s="68" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G41" s="68" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H41" s="68" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="I41" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J41" s="68" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="K41" s="71" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="L41" s="57">
         <f t="shared" ref="L41" si="15">C41*K41</f>
-        <v>0.13</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3938,35 +3962,35 @@
         <v>33</v>
       </c>
       <c r="C42" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" s="67" t="s">
         <v>73</v>
       </c>
       <c r="E42" s="67" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F42" s="69" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G42" s="69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H42" s="69" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="I42" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J42" s="69" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="K42" s="70" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="L42" s="55">
         <f>C42*K42</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3976,35 +4000,35 @@
         <v>34</v>
       </c>
       <c r="C43" s="51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D43" s="68" t="s">
         <v>74</v>
       </c>
       <c r="E43" s="68" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F43" s="68" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G43" s="68" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H43" s="68" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="I43" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J43" s="68" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="K43" s="71" t="s">
-        <v>382</v>
+        <v>409</v>
       </c>
       <c r="L43" s="57">
         <f t="shared" ref="L43" si="16">C43*K43</f>
-        <v>1.1200000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4014,35 +4038,35 @@
         <v>35</v>
       </c>
       <c r="C44" s="50">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D44" s="67" t="s">
         <v>75</v>
       </c>
       <c r="E44" s="67" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F44" s="69" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G44" s="69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H44" s="69" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="I44" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J44" s="69" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="K44" s="70" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="L44" s="55">
         <f>C44*K44</f>
-        <v>0.84</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4052,35 +4076,35 @@
         <v>36</v>
       </c>
       <c r="C45" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D45" s="68" t="s">
         <v>76</v>
       </c>
       <c r="E45" s="68" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F45" s="68" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G45" s="68" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H45" s="68" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="I45" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J45" s="68" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="K45" s="71" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L45" s="57">
         <f t="shared" ref="L45" si="17">C45*K45</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4096,25 +4120,25 @@
         <v>77</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F46" s="69" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G46" s="69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H46" s="69" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="I46" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J46" s="69" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="K46" s="70" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="L46" s="55">
         <f>C46*K46</f>
@@ -4134,67 +4158,67 @@
         <v>78</v>
       </c>
       <c r="E47" s="68" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F47" s="68" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G47" s="68" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="H47" s="68" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="I47" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J47" s="68" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="K47" s="71" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="L47" s="57">
         <f t="shared" ref="L47" si="18">C47*K47</f>
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="3" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
       <c r="B48" s="48">
         <f>ROW(B48) - ROW($B$9)</f>
         <v>39</v>
       </c>
       <c r="C48" s="50">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D48" s="67" t="s">
         <v>79</v>
       </c>
       <c r="E48" s="67" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F48" s="69" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="G48" s="69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H48" s="69" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="I48" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J48" s="69" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="K48" s="70" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="L48" s="55">
         <f>C48*K48</f>
-        <v>4.32</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4204,35 +4228,35 @@
         <v>40</v>
       </c>
       <c r="C49" s="51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D49" s="68" t="s">
         <v>80</v>
       </c>
       <c r="E49" s="68" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F49" s="68" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G49" s="68" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H49" s="68" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="I49" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J49" s="68" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="K49" s="71" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L49" s="57">
         <f t="shared" ref="L49" si="19">C49*K49</f>
-        <v>0.1</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4242,35 +4266,35 @@
         <v>41</v>
       </c>
       <c r="C50" s="50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D50" s="67" t="s">
         <v>81</v>
       </c>
       <c r="E50" s="67" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F50" s="69" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G50" s="69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H50" s="69" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="I50" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J50" s="69" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="K50" s="70" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L50" s="55">
         <f>C50*K50</f>
-        <v>0.30000000000000004</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4280,35 +4304,35 @@
         <v>42</v>
       </c>
       <c r="C51" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" s="68" t="s">
         <v>82</v>
       </c>
       <c r="E51" s="68" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F51" s="68" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G51" s="68" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="H51" s="68" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="I51" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J51" s="68" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="K51" s="71" t="s">
-        <v>383</v>
+        <v>411</v>
       </c>
       <c r="L51" s="57">
         <f t="shared" ref="L51" si="20">C51*K51</f>
-        <v>0.1</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4324,29 +4348,29 @@
         <v>83</v>
       </c>
       <c r="E52" s="67" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F52" s="69" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G52" s="69" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="H52" s="69" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="I52" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J52" s="69" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="K52" s="70" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="L52" s="55">
         <f>C52*K52</f>
-        <v>3.52</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="53" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4362,25 +4386,25 @@
         <v>84</v>
       </c>
       <c r="E53" s="68" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F53" s="68" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G53" s="68" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H53" s="68" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="I53" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J53" s="68" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="K53" s="71" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L53" s="57">
         <f t="shared" ref="L53" si="21">C53*K53</f>
@@ -4394,35 +4418,35 @@
         <v>45</v>
       </c>
       <c r="C54" s="50">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D54" s="67" t="s">
         <v>85</v>
       </c>
       <c r="E54" s="67" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F54" s="69" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G54" s="69" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H54" s="69" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="I54" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J54" s="69" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="K54" s="70" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L54" s="55">
         <f>C54*K54</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="55" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4438,25 +4462,25 @@
         <v>86</v>
       </c>
       <c r="E55" s="68" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F55" s="68" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G55" s="68" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H55" s="68" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="I55" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J55" s="68" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="K55" s="71" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="L55" s="57">
         <f t="shared" ref="L55" si="22">C55*K55</f>
@@ -4470,35 +4494,35 @@
         <v>47</v>
       </c>
       <c r="C56" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56" s="67" t="s">
         <v>87</v>
       </c>
       <c r="E56" s="67" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="F56" s="69" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="G56" s="69" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="H56" s="69" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="I56" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J56" s="69" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="K56" s="70" t="s">
-        <v>383</v>
+        <v>412</v>
       </c>
       <c r="L56" s="55">
         <f>C56*K56</f>
-        <v>0.2</v>
+        <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="57" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4508,35 +4532,35 @@
         <v>48</v>
       </c>
       <c r="C57" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D57" s="68" t="s">
         <v>88</v>
       </c>
       <c r="E57" s="68" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F57" s="68" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G57" s="68" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="H57" s="68" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="I57" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J57" s="68" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="K57" s="71" t="s">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="L57" s="57">
         <f t="shared" ref="L57" si="23">C57*K57</f>
-        <v>2.1800000000000002</v>
+        <v>7.54</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4552,29 +4576,29 @@
         <v>89</v>
       </c>
       <c r="E58" s="67" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="F58" s="69" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G58" s="69" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="H58" s="69" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="I58" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J58" s="69" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="K58" s="70" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="L58" s="55">
         <f>C58*K58</f>
-        <v>7.54</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="59" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4590,29 +4614,29 @@
         <v>90</v>
       </c>
       <c r="E59" s="68" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F59" s="68" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G59" s="68" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="H59" s="68" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="I59" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J59" s="68" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="K59" s="71" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="L59" s="57">
         <f t="shared" ref="L59" si="24">C59*K59</f>
-        <v>2.48</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="60" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4622,35 +4646,35 @@
         <v>51</v>
       </c>
       <c r="C60" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" s="67" t="s">
         <v>91</v>
       </c>
       <c r="E60" s="67" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F60" s="69" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="G60" s="69" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="H60" s="69" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="I60" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J60" s="69" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="K60" s="70" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="L60" s="55">
         <f>C60*K60</f>
-        <v>2.66</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="61" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4666,29 +4690,29 @@
         <v>92</v>
       </c>
       <c r="E61" s="68" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F61" s="68" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G61" s="68" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H61" s="68" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="I61" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J61" s="68" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="K61" s="71" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="L61" s="57">
         <f t="shared" ref="L61" si="25">C61*K61</f>
-        <v>0.48</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="62" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4698,35 +4722,35 @@
         <v>53</v>
       </c>
       <c r="C62" s="50">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D62" s="67" t="s">
         <v>93</v>
       </c>
       <c r="E62" s="67" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F62" s="69" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G62" s="69" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="H62" s="69" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="I62" s="69" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="J62" s="69" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="K62" s="70" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="L62" s="55">
         <f>C62*K62</f>
-        <v>0.25</v>
+        <v>1.6800000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4736,35 +4760,35 @@
         <v>54</v>
       </c>
       <c r="C63" s="51">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D63" s="68" t="s">
         <v>94</v>
       </c>
       <c r="E63" s="68" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F63" s="68" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G63" s="68" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="H63" s="68" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="I63" s="68" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="J63" s="68" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="K63" s="71" t="s">
-        <v>382</v>
+        <v>416</v>
       </c>
       <c r="L63" s="57">
         <f t="shared" ref="L63" si="26">C63*K63</f>
-        <v>2.2400000000000002</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="64" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4774,35 +4798,35 @@
         <v>55</v>
       </c>
       <c r="C64" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D64" s="67" t="s">
         <v>95</v>
       </c>
       <c r="E64" s="67" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F64" s="69" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G64" s="69" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="H64" s="69" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="I64" s="69" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="J64" s="69" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="K64" s="70" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="L64" s="55">
         <f>C64*K64</f>
-        <v>0.97</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="65" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4812,35 +4836,35 @@
         <v>56</v>
       </c>
       <c r="C65" s="51">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D65" s="68" t="s">
         <v>96</v>
       </c>
       <c r="E65" s="68" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F65" s="68" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="G65" s="68" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="H65" s="68" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="I65" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J65" s="68" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="K65" s="71" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="L65" s="57">
         <f t="shared" ref="L65" si="27">C65*K65</f>
-        <v>3.4299999999999997</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4856,29 +4880,29 @@
         <v>97</v>
       </c>
       <c r="E66" s="67" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F66" s="69" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G66" s="69" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="H66" s="69" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="I66" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J66" s="69" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="K66" s="70" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="L66" s="55">
         <f>C66*K66</f>
-        <v>4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="67" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4894,25 +4918,25 @@
         <v>98</v>
       </c>
       <c r="E67" s="68" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F67" s="68" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G67" s="68" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="H67" s="68" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="I67" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J67" s="68" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="K67" s="71" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="L67" s="57">
         <f t="shared" ref="L67" si="28">C67*K67</f>
@@ -4932,25 +4956,25 @@
         <v>99</v>
       </c>
       <c r="E68" s="67" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F68" s="69" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G68" s="69" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="H68" s="69" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="I68" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J68" s="69" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="K68" s="70" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="L68" s="55">
         <f>C68*K68</f>
@@ -4970,25 +4994,25 @@
         <v>100</v>
       </c>
       <c r="E69" s="68" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F69" s="68" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G69" s="68" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="H69" s="68" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="I69" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J69" s="68" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="K69" s="71" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="L69" s="57">
         <f t="shared" ref="L69" si="29">C69*K69</f>
@@ -5008,25 +5032,25 @@
         <v>101</v>
       </c>
       <c r="E70" s="67" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F70" s="69" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G70" s="69" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="H70" s="69" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="I70" s="69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J70" s="69" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="K70" s="70" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="L70" s="55">
         <f>C70*K70</f>
@@ -5046,79 +5070,103 @@
         <v>102</v>
       </c>
       <c r="E71" s="68" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F71" s="68" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="G71" s="68" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="H71" s="68" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="I71" s="68" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="J71" s="68" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="K71" s="71" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="L71" s="57">
         <f t="shared" ref="L71" si="30">C71*K71</f>
+        <v>53.88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="14"/>
+      <c r="B72" s="48">
+        <f>ROW(B72) - ROW($B$9)</f>
+        <v>63</v>
+      </c>
+      <c r="C72" s="50">
+        <v>2</v>
+      </c>
+      <c r="D72" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="E72" s="67" t="s">
+        <v>165</v>
+      </c>
+      <c r="F72" s="69" t="s">
+        <v>229</v>
+      </c>
+      <c r="G72" s="69" t="s">
+        <v>254</v>
+      </c>
+      <c r="H72" s="69" t="s">
+        <v>320</v>
+      </c>
+      <c r="I72" s="69" t="s">
+        <v>322</v>
+      </c>
+      <c r="J72" s="69" t="s">
+        <v>387</v>
+      </c>
+      <c r="K72" s="70" t="s">
+        <v>424</v>
+      </c>
+      <c r="L72" s="55">
+        <f>C72*K72</f>
         <v>1.32</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="58" t="s">
-        <v>19</v>
-      </c>
-      <c r="C72" s="59"/>
-      <c r="D72" s="59"/>
-      <c r="E72" s="47"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J72" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="K72" s="54"/>
-      <c r="L72" s="56">
-        <f>SUM(L10:L71)</f>
-        <v>275.38999999999993</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="14"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
-      <c r="J73" s="8"/>
-      <c r="K73" s="8"/>
-      <c r="L73" s="19"/>
+      <c r="B73" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="47"/>
+      <c r="F73" s="46"/>
+      <c r="G73" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J73" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="K73" s="54"/>
+      <c r="L73" s="56">
+        <f>SUM(L10:L72)</f>
+        <v>328.57999999999987</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="14"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
-      <c r="L74" s="20"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="19"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="14"/>
@@ -5130,30 +5178,39 @@
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
       <c r="I75" s="9"/>
-      <c r="J75" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="J75" s="9"/>
       <c r="K75" s="9"/>
       <c r="L75" s="20"/>
     </row>
-    <row r="76" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="14"/>
-      <c r="B76" s="44"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="16"/>
-      <c r="H76" s="16"/>
-      <c r="I76" s="16"/>
-      <c r="J76" s="16"/>
-      <c r="K76" s="16"/>
-      <c r="L76" s="21"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K76" s="9"/>
+      <c r="L76" s="20"/>
+    </row>
+    <row r="77" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="14"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="16"/>
+      <c r="K77" s="16"/>
+      <c r="L77" s="21"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D79" s="1"/>
@@ -5165,9 +5222,14 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
+    <row r="81" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B73:D73"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.46" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
@@ -5197,7 +5259,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5229,7 +5291,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -5245,7 +5307,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -5269,7 +5331,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="73" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -5277,7 +5339,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="74" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -5285,7 +5347,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="73" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -5293,7 +5355,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="74" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -5301,7 +5363,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="73" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -5309,7 +5371,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -5317,7 +5379,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="73" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REV 3 Files to PCB FAB
</commit_message>
<xml_diff>
--- a/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
+++ b/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{920BB682-B9A5-42C2-A96F-896E15CD7193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87E6181E-56E2-4EE3-8FCB-EF102B751D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,10 +127,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>5/11/2025</t>
-  </si>
-  <si>
-    <t>8:44:53 AM</t>
+    <t>5/12/2025</t>
+  </si>
+  <si>
+    <t>8:55:06 AM</t>
   </si>
   <si>
     <t>Arbitrary Power Booster</t>
@@ -1309,7 +1309,7 @@
     <t>223</t>
   </si>
   <si>
-    <t>5/11/2025 8:44:53 AM</t>
+    <t>5/12/2025 8:55:06 AM</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -2691,11 +2691,11 @@
       </c>
       <c r="E8" s="38">
         <f ca="1">TODAY()</f>
-        <v>45788</v>
+        <v>45789</v>
       </c>
       <c r="F8" s="39">
         <f ca="1">NOW()</f>
-        <v>45788.36558784722</v>
+        <v>45789.372313888889</v>
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>

</xml_diff>

<commit_message>
Hardware modified REV 3 for board outline and cut-outs. Firmware modified the PID struct and how it is called. Added magenta color print. Added Status command to debug. Processor option to printf errors in digital pot driver
</commit_message>
<xml_diff>
--- a/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
+++ b/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87E6181E-56E2-4EE3-8FCB-EF102B751D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{34EFCE36-29B6-404D-9630-9FD793A98BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -127,10 +127,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>5/12/2025</t>
-  </si>
-  <si>
-    <t>8:55:06 AM</t>
+    <t>5/16/2025</t>
+  </si>
+  <si>
+    <t>5:42:46 AM</t>
   </si>
   <si>
     <t>Arbitrary Power Booster</t>
@@ -1309,7 +1309,7 @@
     <t>223</t>
   </si>
   <si>
-    <t>5/12/2025 8:55:06 AM</t>
+    <t>5/16/2025 5:42:46 AM</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -2691,11 +2691,11 @@
       </c>
       <c r="E8" s="38">
         <f ca="1">TODAY()</f>
-        <v>45789</v>
+        <v>45793</v>
       </c>
       <c r="F8" s="39">
         <f ca="1">NOW()</f>
-        <v>45789.372313888889</v>
+        <v>45793.238457175925</v>
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>

</xml_diff>

<commit_message>
Updated schematics to REV 3 PCB stayed at REV 4 - updated output for updated BOM
</commit_message>
<xml_diff>
--- a/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
+++ b/Hardware/Arb_Power_Booster/Default Configuration/Outputs/BOM/BOM_PartType-Arb_Power_Booster.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34EFCE36-29B6-404D-9630-9FD793A98BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59C8D563-63E7-4947-8D11-061530B69C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="461">
   <si>
     <t>Project Full Path</t>
   </si>
@@ -127,10 +127,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>5/16/2025</t>
-  </si>
-  <si>
-    <t>5:42:46 AM</t>
+    <t>5/29/2025</t>
+  </si>
+  <si>
+    <t>9:01:38 AM</t>
   </si>
   <si>
     <t>Arbitrary Power Booster</t>
@@ -139,7 +139,7 @@
     <t>IMR-005-SCH</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
   <si>
     <t>Hab S Collector</t>
@@ -166,6 +166,9 @@
     <t>CAP_SMD_47UF_16V_1210</t>
   </si>
   <si>
+    <t>CAP_SMD_1UF_50V_0805</t>
+  </si>
+  <si>
     <t>CAP_SMD_100UF_25V_SMD</t>
   </si>
   <si>
@@ -235,25 +238,31 @@
     <t>RES_SMD_10K_0805_1/4W_1%</t>
   </si>
   <si>
+    <t>RES_SMD_10K_0805_1/8W_0.1%</t>
+  </si>
+  <si>
     <t>RES_SMD_47K_0805_1/8W_1%</t>
   </si>
   <si>
-    <t>RES_SMD_1.24K_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t>RES_SMD_2.1K_0805_1/8W_1%</t>
+    <t>RES_SMD_1.24K_0805_1/8W_0.1%</t>
+  </si>
+  <si>
+    <t>RES_SMD_2.1K_0805_1/8W_0.1%</t>
   </si>
   <si>
     <t>RES_SMD_0_0805_1/8W_1%</t>
   </si>
   <si>
+    <t>RES_SMD_1.0K_0805_1/8W_0.1%</t>
+  </si>
+  <si>
+    <t>RES_SMD_100K_0805_1/4W_1%</t>
+  </si>
+  <si>
     <t>RES_SMD_1.0K_0805_1/8W_1%</t>
   </si>
   <si>
-    <t>RES_SMD_100K_0805_1/4W_1%</t>
-  </si>
-  <si>
-    <t>RES_SMD_13.7K_0805_1/8W_1%</t>
+    <t>RES_SMD_12.4K_0805_1/8W_1%</t>
   </si>
   <si>
     <t>RES_SMD_300_0805_1/8W_1%</t>
@@ -265,28 +274,34 @@
     <t>RES_SMD_100_0805_3.5W_1%</t>
   </si>
   <si>
-    <t>RES_SMD_1.5K_0805_1/8W_1%</t>
+    <t>RES_SMD_1.5K_0805_1/8W_0.1%</t>
+  </si>
+  <si>
+    <t>RES_SMD_4.7K_0805_1/8W_0.1%</t>
+  </si>
+  <si>
+    <t>RES_SMD_90.9_0805_1/8W_1%</t>
+  </si>
+  <si>
+    <t>RES_SMD_0.0065_2512_2W_1%</t>
+  </si>
+  <si>
+    <t>RES_SMD_3.0K_0805_1/8W_0.1%</t>
+  </si>
+  <si>
+    <t>RES_SMD_4.99K_0805_1/8W_1%</t>
+  </si>
+  <si>
+    <t>RES_SMD_2.49K_0805_1/8W_1%</t>
+  </si>
+  <si>
+    <t>RES_SMD_5.0K_0805_1/8W_0.1%</t>
   </si>
   <si>
     <t>RES_SMD_4.7K_0805_1/8W_1%</t>
   </si>
   <si>
-    <t>RES_SMD_90.9_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t>RES_SMD_0.0065_2512_2W_1%</t>
-  </si>
-  <si>
-    <t>RES_SMD_3.0K_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t>RES_SMD_4.99K_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t>RES_SMD_2.49K_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t>RES_SMD_100_0805_1/8W_1%</t>
+    <t>RES_SMD_10_0805_1/8W_1%</t>
   </si>
   <si>
     <t>RELAY_AZ733-2AE-5DE</t>
@@ -358,6 +373,9 @@
     <t>CAP CER 47UF 50V X5R 1210</t>
   </si>
   <si>
+    <t>CAP CER 1UF 50V X7R 0805</t>
+  </si>
+  <si>
     <t>CAP CER 100UF 25V X7S SMD</t>
   </si>
   <si>
@@ -427,25 +445,31 @@
     <t>RES SMD 10K OHM 1% 1/4W 0805</t>
   </si>
   <si>
+    <t>RES SMD 10K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
     <t>RES SMD 47K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>RES SMD 1.24K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD 2.1K OHM 1% 1/8W 0805</t>
+    <t>RES SMD 1.24K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 2.1K OHM 0.1% 1/8W 0805</t>
   </si>
   <si>
     <t>RES SMD 0 OHM 1% 1/8W 0805</t>
   </si>
   <si>
+    <t>RES SMD 1.0K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
     <t>RES SMD 1.0K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>RES SMD 100K OHM 1% 1/4W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD 13.7K OHM 1% 1/8W 0805</t>
+    <t>RES SMD 12.4K OHM 1% 1/8W 0805</t>
   </si>
   <si>
     <t>RES SMD 300 OHM 1% 1/8W 0805</t>
@@ -457,28 +481,34 @@
     <t>RES SMD 100 OHM 1% 3.5W 2512</t>
   </si>
   <si>
-    <t>RES SMD 1.5K OHM 1% 1/8W 0805</t>
+    <t>RES SMD 1.5K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 90.9 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0065 OHM 1% 2W 2512</t>
+  </si>
+  <si>
+    <t>RES SMD 3.0K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 4.99K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 2.49K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 5.0K OHM 0.1% 1/8W 0805</t>
   </si>
   <si>
     <t>RES SMD 4.7K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>RES SMD 90.9 OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD 0.0065 OHM 1% 2W 2512</t>
-  </si>
-  <si>
-    <t>RES SMD 3.0K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD 4.99K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD 2.49K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD 100 OHM 1% 1/8W 0805</t>
+    <t>RES SMD 10 OHM 1% 1/8W 0805</t>
   </si>
   <si>
     <t>RELAY GEN PURPOSE SPDT 10A 5V</t>
@@ -535,7 +565,7 @@
     <t>C4, C12, C16</t>
   </si>
   <si>
-    <t>C5, C6, C7, C8, C13, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46</t>
+    <t>C5, C6, C7, C8, C13, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C29, C33, C34, C35, C36, C37, C38, C39, C40, C41, C43, C44, C45, C46</t>
   </si>
   <si>
     <t>C14</t>
@@ -544,6 +574,9 @@
     <t>C15, C48</t>
   </si>
   <si>
+    <t>C28, C42</t>
+  </si>
+  <si>
     <t>C30, C31, C32, C47</t>
   </si>
   <si>
@@ -610,7 +643,10 @@
     <t>R1, R6</t>
   </si>
   <si>
-    <t>R2, R3, R7, R8, R11, R25, R27, R30, R31, R32, R37, R38, R42, R43, R45, R46, R47, R51, R52, R53, R54, R61, R62, R63, R64, R65, R66, R67, R69, R72</t>
+    <t>R2, R7, R8, R25, R27, R30, R31, R32, R37, R38, R45, R51, R52, R63, R65, R66, R67, R69</t>
+  </si>
+  <si>
+    <t>R3, R11, R42, R43, R46, R47, R53, R54, R61, R62, R64, R72</t>
   </si>
   <si>
     <t>R4, R13</t>
@@ -625,12 +661,15 @@
     <t>R10, R18, R19, R24, R26, R28, R36, R50</t>
   </si>
   <si>
-    <t>R12, R16</t>
+    <t>R12</t>
   </si>
   <si>
     <t>R14</t>
   </si>
   <si>
+    <t>R16</t>
+  </si>
+  <si>
     <t>R17</t>
   </si>
   <si>
@@ -646,7 +685,7 @@
     <t>R33</t>
   </si>
   <si>
-    <t>R34, R60, R70</t>
+    <t>R34</t>
   </si>
   <si>
     <t>R35</t>
@@ -658,12 +697,18 @@
     <t>R40, R49</t>
   </si>
   <si>
-    <t>R41, R48, R55, R68</t>
+    <t>R41, R48</t>
   </si>
   <si>
     <t>R44, R56</t>
   </si>
   <si>
+    <t>R55, R68</t>
+  </si>
+  <si>
+    <t>R60, R70</t>
+  </si>
+  <si>
     <t>R73, R74</t>
   </si>
   <si>
@@ -817,6 +862,9 @@
     <t>GRM32ER60J476ME20L</t>
   </si>
   <si>
+    <t>08055C105K4T2A</t>
+  </si>
+  <si>
     <t>KCM55WC71E107MH13L</t>
   </si>
   <si>
@@ -886,25 +934,31 @@
     <t>RC0805FR-7W10KL</t>
   </si>
   <si>
+    <t>RP0805BRD0710KL</t>
+  </si>
+  <si>
     <t>RC0805FR-1347KL</t>
   </si>
   <si>
-    <t>RC0805FR-071K24L</t>
-  </si>
-  <si>
-    <t>RC0805FR-072K1L</t>
+    <t>RT0805BRD071K24L</t>
+  </si>
+  <si>
+    <t>RT0805BRD072K1L</t>
   </si>
   <si>
     <t>RC0805JR-070RL</t>
   </si>
   <si>
+    <t>RT0805BRD071KL</t>
+  </si>
+  <si>
+    <t>RC0805FR-07100KL</t>
+  </si>
+  <si>
     <t>RC0805FR-071KL</t>
   </si>
   <si>
-    <t>RC0805FR-07100KL</t>
-  </si>
-  <si>
-    <t>RC0805FR-0713K7L</t>
+    <t>RC0805FR-0712K4L</t>
   </si>
   <si>
     <t>RC0805FR-07300RL</t>
@@ -916,28 +970,34 @@
     <t>ALN2512F100RE-1</t>
   </si>
   <si>
-    <t>RC0805FR-071K5L</t>
+    <t>RT0805BRD071K5L</t>
+  </si>
+  <si>
+    <t>RT0805BRD074K7L</t>
+  </si>
+  <si>
+    <t>RC0805FR-0790R9L</t>
+  </si>
+  <si>
+    <t>WSL25126L500FEA18</t>
+  </si>
+  <si>
+    <t>RT0805BRD073KL</t>
+  </si>
+  <si>
+    <t>RC0805FR-134K99L</t>
+  </si>
+  <si>
+    <t>RC0805FR-132K49L</t>
+  </si>
+  <si>
+    <t>AT0805BRD075KL</t>
   </si>
   <si>
     <t>RC0805FR-134K7L</t>
   </si>
   <si>
-    <t>RC0805FR-0790R9L</t>
-  </si>
-  <si>
-    <t>WSL25126L500FEA18</t>
-  </si>
-  <si>
-    <t>RC0805FR-133KL</t>
-  </si>
-  <si>
-    <t>RC0805FR-134K99L</t>
-  </si>
-  <si>
-    <t>RC0805FR-132K49L</t>
-  </si>
-  <si>
-    <t>RC0805FR-07100RL</t>
+    <t>RC0805FR-1310RL</t>
   </si>
   <si>
     <t>AZ733-2AE-5DE</t>
@@ -1018,6 +1078,9 @@
     <t>490-1887-1-ND</t>
   </si>
   <si>
+    <t>478-KAM21KR71H105KUCT-ND</t>
+  </si>
+  <si>
     <t>490-KCM55WC71E107MH13LCT-ND</t>
   </si>
   <si>
@@ -1087,25 +1150,31 @@
     <t>13-RC0805FR-7W10KLCT-ND</t>
   </si>
   <si>
+    <t>13-RP0805BRD0710KLCT-ND</t>
+  </si>
+  <si>
     <t>13-RC0805FR-1347KLCT-ND</t>
   </si>
   <si>
-    <t>311-1.24KCRCT-ND</t>
-  </si>
-  <si>
-    <t>311-2.10KCRCT-ND</t>
+    <t>YAG1809CT-ND</t>
+  </si>
+  <si>
+    <t>YAG1852CT-ND</t>
   </si>
   <si>
     <t>311-0.0ARCT-ND</t>
   </si>
   <si>
+    <t>YAG1820CT-ND</t>
+  </si>
+  <si>
+    <t>311-100KCRCT-ND</t>
+  </si>
+  <si>
     <t>311-1.00KCRCT-ND</t>
   </si>
   <si>
-    <t>311-100KCRCT-ND</t>
-  </si>
-  <si>
-    <t>311-13.7KCRCT-ND</t>
+    <t>311-12.4KCRCT-ND</t>
   </si>
   <si>
     <t>311-300CRCT-ND</t>
@@ -1117,28 +1186,34 @@
     <t>273-ALN2512F100RE-1CT-ND</t>
   </si>
   <si>
-    <t>311-1.50KCRCT-ND</t>
+    <t>YAG1814CT-ND</t>
+  </si>
+  <si>
+    <t>YAG1919CT-ND</t>
+  </si>
+  <si>
+    <t>311-90.9CRCT-ND</t>
+  </si>
+  <si>
+    <t>541-WSL25126L500FEA18CT-ND</t>
+  </si>
+  <si>
+    <t>YAG1891CT-ND</t>
+  </si>
+  <si>
+    <t>13-RC0805FR-134K99LCT-ND</t>
+  </si>
+  <si>
+    <t>13-RC0805FR-132K49LCT-ND</t>
+  </si>
+  <si>
+    <t>13-AT0805BRD075KLCT-ND</t>
   </si>
   <si>
     <t>13-RC0805FR-134K7LCT-ND</t>
   </si>
   <si>
-    <t>311-90.9CRCT-ND</t>
-  </si>
-  <si>
-    <t>541-WSL25126L500FEA18CT-ND</t>
-  </si>
-  <si>
-    <t>13-RC0805FR-133KLCT-ND</t>
-  </si>
-  <si>
-    <t>13-RC0805FR-134K99LCT-ND</t>
-  </si>
-  <si>
-    <t>13-RC0805FR-132K49LCT-ND</t>
-  </si>
-  <si>
-    <t>311-100CRCT-ND</t>
+    <t>13-RC0805FR-1310RLCT-ND</t>
   </si>
   <si>
     <t>3385-AZ733-2AE-5DE-nd</t>
@@ -1207,6 +1282,9 @@
     <t>.24</t>
   </si>
   <si>
+    <t>.27</t>
+  </si>
+  <si>
     <t>5.68</t>
   </si>
   <si>
@@ -1264,6 +1342,12 @@
     <t>1.76</t>
   </si>
   <si>
+    <t>0.16</t>
+  </si>
+  <si>
+    <t>.56</t>
+  </si>
+  <si>
     <t>2.18</t>
   </si>
   <si>
@@ -1309,7 +1393,7 @@
     <t>223</t>
   </si>
   <si>
-    <t>5/16/2025 5:42:46 AM</t>
+    <t>5/29/2025 9:01:38 AM</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -2530,7 +2614,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -2691,11 +2775,11 @@
       </c>
       <c r="E8" s="38">
         <f ca="1">TODAY()</f>
-        <v>45793</v>
+        <v>45806</v>
       </c>
       <c r="F8" s="39">
         <f ca="1">NOW()</f>
-        <v>45793.238457175925</v>
+        <v>45806.376862500001</v>
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>
@@ -2715,25 +2799,25 @@
         <v>40</v>
       </c>
       <c r="E9" s="66" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="G9" s="66" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="H9" s="66" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="I9" s="66" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="J9" s="66" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="K9" s="66" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="L9" s="25" t="s">
         <v>29</v>
@@ -2752,25 +2836,25 @@
         <v>41</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F10" s="69" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="G10" s="69" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="H10" s="69" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="I10" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J10" s="69" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="K10" s="70" t="s">
-        <v>389</v>
+        <v>414</v>
       </c>
       <c r="L10" s="55">
         <f>C10*K10</f>
@@ -2790,28 +2874,28 @@
         <v>42</v>
       </c>
       <c r="E11" s="68" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F11" s="68" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="G11" s="68" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="H11" s="68" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="I11" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J11" s="68" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="K11" s="71" t="s">
-        <v>390</v>
+        <v>415</v>
       </c>
       <c r="L11" s="57">
-        <f t="shared" ref="L11:L72" si="0">C11*K11</f>
+        <f t="shared" ref="L11:L77" si="0">C11*K11</f>
         <v>0.84000000000000008</v>
       </c>
     </row>
@@ -2822,35 +2906,35 @@
         <v>3</v>
       </c>
       <c r="C12" s="50">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D12" s="67" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F12" s="69" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="G12" s="69" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="H12" s="69" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="I12" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J12" s="69" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
       <c r="K12" s="70" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="L12" s="55">
         <f>C12*K12</f>
-        <v>3.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2866,25 +2950,25 @@
         <v>44</v>
       </c>
       <c r="E13" s="68" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F13" s="68" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="G13" s="68" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="H13" s="68" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="I13" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J13" s="68" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
       <c r="K13" s="71" t="s">
-        <v>392</v>
+        <v>417</v>
       </c>
       <c r="L13" s="57">
         <f t="shared" ref="L13" si="1">C13*K13</f>
@@ -2904,25 +2988,25 @@
         <v>45</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F14" s="69" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="G14" s="69" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="H14" s="69" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="I14" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J14" s="69" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
       <c r="K14" s="70" t="s">
-        <v>390</v>
+        <v>415</v>
       </c>
       <c r="L14" s="55">
         <f>C14*K14</f>
@@ -2936,73 +3020,73 @@
         <v>6</v>
       </c>
       <c r="C15" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" s="68" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F15" s="68" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="G15" s="68" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="H15" s="68" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="I15" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J15" s="68" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="K15" s="71" t="s">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="L15" s="57">
         <f t="shared" ref="L15" si="2">C15*K15</f>
-        <v>22.72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="48">
         <f>ROW(B16) - ROW($B$9)</f>
         <v>7</v>
       </c>
       <c r="C16" s="50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16" s="67" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F16" s="69" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="G16" s="69" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="H16" s="69" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="I16" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J16" s="69" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="K16" s="70" t="s">
-        <v>394</v>
+        <v>419</v>
       </c>
       <c r="L16" s="55">
         <f>C16*K16</f>
-        <v>0.36</v>
+        <v>22.72</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3012,73 +3096,73 @@
         <v>8</v>
       </c>
       <c r="C17" s="51">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D17" s="68" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="68" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F17" s="68" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="G17" s="68" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="H17" s="68" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="I17" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J17" s="68" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="K17" s="71" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
       <c r="L17" s="57">
         <f t="shared" ref="L17" si="3">C17*K17</f>
-        <v>2.72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="3" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="48">
         <f>ROW(B18) - ROW($B$9)</f>
         <v>9</v>
       </c>
       <c r="C18" s="50">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D18" s="67" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="F18" s="69" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="G18" s="69" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="H18" s="69" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="I18" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J18" s="69" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="K18" s="70" t="s">
-        <v>396</v>
+        <v>421</v>
       </c>
       <c r="L18" s="55">
         <f>C18*K18</f>
-        <v>0.5</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3088,35 +3172,35 @@
         <v>10</v>
       </c>
       <c r="C19" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="68" t="s">
         <v>50</v>
       </c>
       <c r="E19" s="68" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F19" s="68" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="G19" s="68" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="H19" s="68" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="I19" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J19" s="68" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="K19" s="71" t="s">
-        <v>396</v>
+        <v>422</v>
       </c>
       <c r="L19" s="57">
         <f t="shared" ref="L19" si="4">C19*K19</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3126,35 +3210,35 @@
         <v>11</v>
       </c>
       <c r="C20" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="67" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="67" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F20" s="69" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G20" s="69" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="H20" s="69" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="I20" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J20" s="69" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="K20" s="70" t="s">
-        <v>397</v>
+        <v>422</v>
       </c>
       <c r="L20" s="55">
         <f>C20*K20</f>
-        <v>14.62</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3164,35 +3248,35 @@
         <v>12</v>
       </c>
       <c r="C21" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E21" s="68" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F21" s="68" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="G21" s="68" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="H21" s="68" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="I21" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J21" s="68" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="K21" s="71" t="s">
-        <v>398</v>
+        <v>423</v>
       </c>
       <c r="L21" s="57">
         <f t="shared" ref="L21" si="5">C21*K21</f>
-        <v>0.1</v>
+        <v>14.62</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3202,35 +3286,35 @@
         <v>13</v>
       </c>
       <c r="C22" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="67" t="s">
         <v>53</v>
       </c>
       <c r="E22" s="67" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="F22" s="69" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="G22" s="69" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="H22" s="69" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="I22" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J22" s="69" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="K22" s="70" t="s">
-        <v>399</v>
+        <v>424</v>
       </c>
       <c r="L22" s="55">
         <f>C22*K22</f>
-        <v>6.82</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3240,35 +3324,35 @@
         <v>14</v>
       </c>
       <c r="C23" s="51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23" s="68" t="s">
         <v>54</v>
       </c>
       <c r="E23" s="68" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="F23" s="68" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="G23" s="68" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="H23" s="68" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="I23" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J23" s="68" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="K23" s="71" t="s">
-        <v>400</v>
+        <v>425</v>
       </c>
       <c r="L23" s="57">
         <f t="shared" ref="L23" si="6">C23*K23</f>
-        <v>41.56</v>
+        <v>6.82</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3284,25 +3368,25 @@
         <v>55</v>
       </c>
       <c r="E24" s="67" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F24" s="69" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G24" s="69" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="H24" s="69" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="I24" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J24" s="69" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="K24" s="70" t="s">
-        <v>400</v>
+        <v>426</v>
       </c>
       <c r="L24" s="55">
         <f>C24*K24</f>
@@ -3316,35 +3400,35 @@
         <v>16</v>
       </c>
       <c r="C25" s="51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D25" s="68" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="68" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F25" s="68" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="G25" s="68" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="H25" s="68" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="I25" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J25" s="68" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="K25" s="71" t="s">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="L25" s="57">
         <f t="shared" ref="L25" si="7">C25*K25</f>
-        <v>2.8</v>
+        <v>41.56</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3354,35 +3438,35 @@
         <v>17</v>
       </c>
       <c r="C26" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="67" t="s">
         <v>57</v>
       </c>
       <c r="E26" s="67" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="F26" s="69" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="G26" s="69" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="H26" s="69" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="I26" s="69" t="s">
-        <v>323</v>
+        <v>342</v>
       </c>
       <c r="J26" s="69" t="s">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="K26" s="70" t="s">
-        <v>402</v>
+        <v>427</v>
       </c>
       <c r="L26" s="55">
         <f>C26*K26</f>
-        <v>7.0000000000000007E-2</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3392,35 +3476,35 @@
         <v>18</v>
       </c>
       <c r="C27" s="51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D27" s="68" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F27" s="68" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="G27" s="68" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="H27" s="68" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="I27" s="68" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="J27" s="68" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="K27" s="71" t="s">
-        <v>402</v>
+        <v>428</v>
       </c>
       <c r="L27" s="57">
         <f t="shared" ref="L27" si="8">C27*K27</f>
-        <v>0.28000000000000003</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3430,35 +3514,35 @@
         <v>19</v>
       </c>
       <c r="C28" s="50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D28" s="67" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="67" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F28" s="69" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="G28" s="69" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="H28" s="69" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="I28" s="69" t="s">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c r="J28" s="69" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
       <c r="K28" s="70" t="s">
-        <v>403</v>
+        <v>428</v>
       </c>
       <c r="L28" s="55">
         <f>C28*K28</f>
-        <v>0.48</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3468,73 +3552,73 @@
         <v>20</v>
       </c>
       <c r="C29" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" s="68" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="68" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F29" s="68" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="G29" s="68" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="H29" s="68" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="I29" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J29" s="68" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="K29" s="71" t="s">
-        <v>394</v>
+        <v>429</v>
       </c>
       <c r="L29" s="57">
         <f t="shared" ref="L29" si="9">C29*K29</f>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="3" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="48">
         <f>ROW(B30) - ROW($B$9)</f>
         <v>21</v>
       </c>
       <c r="C30" s="50">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D30" s="67" t="s">
         <v>61</v>
       </c>
       <c r="E30" s="67" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="F30" s="69" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="G30" s="69" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="H30" s="69" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
       <c r="I30" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J30" s="69" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="K30" s="70" t="s">
-        <v>404</v>
+        <v>420</v>
       </c>
       <c r="L30" s="55">
         <f>C30*K30</f>
-        <v>4.6399999999999997</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3544,35 +3628,35 @@
         <v>22</v>
       </c>
       <c r="C31" s="51">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D31" s="68" t="s">
         <v>62</v>
       </c>
       <c r="E31" s="68" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="F31" s="68" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="G31" s="68" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="H31" s="68" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="I31" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J31" s="68" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="K31" s="71" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="L31" s="57">
         <f t="shared" ref="L31" si="10">C31*K31</f>
-        <v>5.44</v>
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3582,35 +3666,35 @@
         <v>23</v>
       </c>
       <c r="C32" s="50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D32" s="67" t="s">
         <v>63</v>
       </c>
       <c r="E32" s="67" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="F32" s="69" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="G32" s="69" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="H32" s="69" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="I32" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J32" s="69" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="K32" s="70" t="s">
-        <v>406</v>
+        <v>431</v>
       </c>
       <c r="L32" s="55">
         <f>C32*K32</f>
-        <v>2.14</v>
+        <v>5.44</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3620,73 +3704,73 @@
         <v>24</v>
       </c>
       <c r="C33" s="51">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D33" s="68" t="s">
         <v>64</v>
       </c>
       <c r="E33" s="68" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F33" s="68" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="G33" s="68" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="H33" s="68" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="I33" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J33" s="68" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="K33" s="71" t="s">
-        <v>407</v>
+        <v>432</v>
       </c>
       <c r="L33" s="57">
         <f t="shared" ref="L33" si="11">C33*K33</f>
-        <v>1.4000000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14"/>
       <c r="B34" s="48">
         <f>ROW(B34) - ROW($B$9)</f>
         <v>25</v>
       </c>
       <c r="C34" s="50">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D34" s="67" t="s">
         <v>65</v>
       </c>
       <c r="E34" s="67" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F34" s="69" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="G34" s="69" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="H34" s="69" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="I34" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J34" s="69" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="K34" s="70" t="s">
-        <v>405</v>
+        <v>433</v>
       </c>
       <c r="L34" s="55">
         <f>C34*K34</f>
-        <v>1.36</v>
+        <v>1.4000000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3696,35 +3780,35 @@
         <v>26</v>
       </c>
       <c r="C35" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="68" t="s">
         <v>66</v>
       </c>
       <c r="E35" s="68" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F35" s="68" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="G35" s="68" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="H35" s="68" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="I35" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J35" s="68" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="K35" s="71" t="s">
-        <v>403</v>
+        <v>431</v>
       </c>
       <c r="L35" s="57">
         <f t="shared" ref="L35" si="12">C35*K35</f>
-        <v>0.96</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3740,29 +3824,29 @@
         <v>67</v>
       </c>
       <c r="E36" s="67" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F36" s="69" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="G36" s="69" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="H36" s="69" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="I36" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J36" s="69" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="K36" s="70" t="s">
-        <v>408</v>
+        <v>429</v>
       </c>
       <c r="L36" s="55">
         <f>C36*K36</f>
-        <v>0.4</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3772,73 +3856,73 @@
         <v>28</v>
       </c>
       <c r="C37" s="51">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D37" s="68" t="s">
         <v>68</v>
       </c>
       <c r="E37" s="68" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F37" s="68" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="G37" s="68" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H37" s="68" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="I37" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J37" s="68" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="K37" s="71" t="s">
-        <v>398</v>
+        <v>434</v>
       </c>
       <c r="L37" s="57">
         <f t="shared" ref="L37" si="13">C37*K37</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="3" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
       <c r="B38" s="48">
         <f>ROW(B38) - ROW($B$9)</f>
         <v>29</v>
       </c>
       <c r="C38" s="50">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D38" s="67" t="s">
         <v>69</v>
       </c>
       <c r="E38" s="67" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F38" s="69" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="G38" s="69" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H38" s="69" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="I38" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J38" s="69" t="s">
-        <v>353</v>
+        <v>373</v>
       </c>
       <c r="K38" s="70" t="s">
-        <v>391</v>
+        <v>424</v>
       </c>
       <c r="L38" s="55">
         <f>C38*K38</f>
-        <v>0.2</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3848,35 +3932,35 @@
         <v>30</v>
       </c>
       <c r="C39" s="51">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D39" s="68" t="s">
         <v>70</v>
       </c>
       <c r="E39" s="68" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F39" s="68" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="G39" s="68" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H39" s="68" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="I39" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J39" s="68" t="s">
-        <v>354</v>
+        <v>374</v>
       </c>
       <c r="K39" s="71" t="s">
-        <v>391</v>
+        <v>421</v>
       </c>
       <c r="L39" s="57">
         <f t="shared" ref="L39" si="14">C39*K39</f>
-        <v>0.2</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3886,35 +3970,35 @@
         <v>31</v>
       </c>
       <c r="C40" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="67" t="s">
         <v>71</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F40" s="69" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="G40" s="69" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H40" s="69" t="s">
-        <v>288</v>
+        <v>303</v>
       </c>
       <c r="I40" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J40" s="69" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="K40" s="70" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="L40" s="55">
         <f>C40*K40</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3924,35 +4008,35 @@
         <v>32</v>
       </c>
       <c r="C41" s="51">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D41" s="68" t="s">
         <v>72</v>
       </c>
       <c r="E41" s="68" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F41" s="68" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="G41" s="68" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H41" s="68" t="s">
-        <v>289</v>
+        <v>304</v>
       </c>
       <c r="I41" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J41" s="68" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="K41" s="71" t="s">
-        <v>391</v>
+        <v>421</v>
       </c>
       <c r="L41" s="57">
         <f t="shared" ref="L41" si="15">C41*K41</f>
-        <v>0.8</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3962,35 +4046,35 @@
         <v>33</v>
       </c>
       <c r="C42" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="67" t="s">
         <v>73</v>
       </c>
       <c r="E42" s="67" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F42" s="69" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="G42" s="69" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H42" s="69" t="s">
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="I42" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J42" s="69" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="K42" s="70" t="s">
-        <v>391</v>
+        <v>421</v>
       </c>
       <c r="L42" s="55">
         <f>C42*K42</f>
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4000,35 +4084,35 @@
         <v>34</v>
       </c>
       <c r="C43" s="51">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D43" s="68" t="s">
         <v>74</v>
       </c>
       <c r="E43" s="68" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="F43" s="68" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="G43" s="68" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H43" s="68" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="I43" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J43" s="68" t="s">
-        <v>358</v>
+        <v>378</v>
       </c>
       <c r="K43" s="71" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="L43" s="57">
         <f t="shared" ref="L43" si="16">C43*K43</f>
-        <v>0.13</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4044,29 +4128,29 @@
         <v>75</v>
       </c>
       <c r="E44" s="67" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F44" s="69" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="G44" s="69" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H44" s="69" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="I44" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J44" s="69" t="s">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="K44" s="70" t="s">
-        <v>398</v>
+        <v>421</v>
       </c>
       <c r="L44" s="55">
         <f>C44*K44</f>
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4076,35 +4160,35 @@
         <v>36</v>
       </c>
       <c r="C45" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" s="68" t="s">
         <v>76</v>
       </c>
       <c r="E45" s="68" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F45" s="68" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="G45" s="68" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H45" s="68" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="I45" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J45" s="68" t="s">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="K45" s="71" t="s">
-        <v>391</v>
+        <v>435</v>
       </c>
       <c r="L45" s="57">
         <f t="shared" ref="L45" si="17">C45*K45</f>
-        <v>0.2</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4114,35 +4198,35 @@
         <v>37</v>
       </c>
       <c r="C46" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D46" s="67" t="s">
         <v>77</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F46" s="69" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="G46" s="69" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H46" s="69" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
       <c r="I46" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J46" s="69" t="s">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="K46" s="70" t="s">
-        <v>398</v>
+        <v>416</v>
       </c>
       <c r="L46" s="55">
         <f>C46*K46</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="47" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4152,35 +4236,35 @@
         <v>38</v>
       </c>
       <c r="C47" s="51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D47" s="68" t="s">
         <v>78</v>
       </c>
       <c r="E47" s="68" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F47" s="68" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="G47" s="68" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="H47" s="68" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="I47" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J47" s="68" t="s">
-        <v>362</v>
+        <v>382</v>
       </c>
       <c r="K47" s="71" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="L47" s="57">
         <f t="shared" ref="L47" si="18">C47*K47</f>
-        <v>6</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4190,35 +4274,35 @@
         <v>39</v>
       </c>
       <c r="C48" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48" s="67" t="s">
         <v>79</v>
       </c>
       <c r="E48" s="67" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F48" s="69" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G48" s="69" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H48" s="69" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="I48" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J48" s="69" t="s">
-        <v>363</v>
+        <v>383</v>
       </c>
       <c r="K48" s="70" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="L48" s="55">
         <f>C48*K48</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4228,35 +4312,35 @@
         <v>40</v>
       </c>
       <c r="C49" s="51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D49" s="68" t="s">
         <v>80</v>
       </c>
       <c r="E49" s="68" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F49" s="68" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="G49" s="68" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H49" s="68" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
       <c r="I49" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J49" s="68" t="s">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="K49" s="71" t="s">
-        <v>391</v>
+        <v>424</v>
       </c>
       <c r="L49" s="57">
         <f t="shared" ref="L49" si="19">C49*K49</f>
-        <v>0.30000000000000004</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4266,35 +4350,35 @@
         <v>41</v>
       </c>
       <c r="C50" s="50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D50" s="67" t="s">
         <v>81</v>
       </c>
       <c r="E50" s="67" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F50" s="69" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="G50" s="69" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="H50" s="69" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="I50" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J50" s="69" t="s">
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K50" s="70" t="s">
-        <v>391</v>
+        <v>436</v>
       </c>
       <c r="L50" s="55">
         <f>C50*K50</f>
-        <v>0.1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4304,35 +4388,35 @@
         <v>42</v>
       </c>
       <c r="C51" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" s="68" t="s">
         <v>82</v>
       </c>
       <c r="E51" s="68" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="F51" s="68" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="G51" s="68" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="H51" s="68" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
       <c r="I51" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J51" s="68" t="s">
-        <v>366</v>
+        <v>386</v>
       </c>
       <c r="K51" s="71" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="L51" s="57">
         <f t="shared" ref="L51" si="20">C51*K51</f>
-        <v>3.52</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4342,35 +4426,35 @@
         <v>43</v>
       </c>
       <c r="C52" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52" s="67" t="s">
         <v>83</v>
       </c>
       <c r="E52" s="67" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="F52" s="69" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="G52" s="69" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H52" s="69" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="I52" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J52" s="69" t="s">
-        <v>367</v>
+        <v>387</v>
       </c>
       <c r="K52" s="70" t="s">
-        <v>391</v>
+        <v>421</v>
       </c>
       <c r="L52" s="55">
         <f>C52*K52</f>
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="53" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4380,35 +4464,35 @@
         <v>44</v>
       </c>
       <c r="C53" s="51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D53" s="68" t="s">
         <v>84</v>
       </c>
       <c r="E53" s="68" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F53" s="68" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="G53" s="68" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H53" s="68" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="I53" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J53" s="68" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="K53" s="71" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="L53" s="57">
         <f t="shared" ref="L53" si="21">C53*K53</f>
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4424,29 +4508,29 @@
         <v>85</v>
       </c>
       <c r="E54" s="67" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="F54" s="69" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="G54" s="69" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="H54" s="69" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="I54" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J54" s="69" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="K54" s="70" t="s">
-        <v>391</v>
+        <v>437</v>
       </c>
       <c r="L54" s="55">
         <f>C54*K54</f>
-        <v>0.2</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="55" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4462,29 +4546,29 @@
         <v>86</v>
       </c>
       <c r="E55" s="68" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F55" s="68" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="G55" s="68" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H55" s="68" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="I55" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J55" s="68" t="s">
-        <v>370</v>
+        <v>390</v>
       </c>
       <c r="K55" s="71" t="s">
-        <v>391</v>
+        <v>438</v>
       </c>
       <c r="L55" s="57">
         <f t="shared" ref="L55" si="22">C55*K55</f>
-        <v>0.2</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="56" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4494,35 +4578,35 @@
         <v>47</v>
       </c>
       <c r="C56" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" s="67" t="s">
         <v>87</v>
       </c>
       <c r="E56" s="67" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="F56" s="69" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="G56" s="69" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="H56" s="69" t="s">
-        <v>304</v>
+        <v>319</v>
       </c>
       <c r="I56" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J56" s="69" t="s">
-        <v>371</v>
+        <v>391</v>
       </c>
       <c r="K56" s="70" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="L56" s="55">
         <f>C56*K56</f>
-        <v>2.1800000000000002</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="57" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4538,29 +4622,29 @@
         <v>88</v>
       </c>
       <c r="E57" s="68" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="F57" s="68" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="G57" s="68" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="H57" s="68" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="I57" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J57" s="68" t="s">
-        <v>372</v>
+        <v>392</v>
       </c>
       <c r="K57" s="71" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="L57" s="57">
         <f t="shared" ref="L57" si="23">C57*K57</f>
-        <v>7.54</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4576,29 +4660,29 @@
         <v>89</v>
       </c>
       <c r="E58" s="67" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="F58" s="69" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="G58" s="69" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="H58" s="69" t="s">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="I58" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J58" s="69" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="K58" s="70" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
       <c r="L58" s="55">
         <f>C58*K58</f>
-        <v>2.48</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4614,29 +4698,29 @@
         <v>90</v>
       </c>
       <c r="E59" s="68" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="F59" s="68" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="G59" s="68" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="H59" s="68" t="s">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="I59" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J59" s="68" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="K59" s="71" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="L59" s="57">
         <f t="shared" ref="L59" si="24">C59*K59</f>
-        <v>2.66</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="60" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4646,35 +4730,35 @@
         <v>51</v>
       </c>
       <c r="C60" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" s="67" t="s">
         <v>91</v>
       </c>
       <c r="E60" s="67" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="F60" s="69" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="G60" s="69" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="H60" s="69" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="I60" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J60" s="69" t="s">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="K60" s="70" t="s">
-        <v>403</v>
+        <v>416</v>
       </c>
       <c r="L60" s="55">
         <f>C60*K60</f>
-        <v>0.48</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="61" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4690,29 +4774,29 @@
         <v>92</v>
       </c>
       <c r="E61" s="68" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="F61" s="68" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="G61" s="68" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="H61" s="68" t="s">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="I61" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J61" s="68" t="s">
-        <v>376</v>
+        <v>396</v>
       </c>
       <c r="K61" s="71" t="s">
-        <v>396</v>
+        <v>440</v>
       </c>
       <c r="L61" s="57">
         <f t="shared" ref="L61" si="25">C61*K61</f>
-        <v>0.25</v>
+        <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4722,35 +4806,35 @@
         <v>53</v>
       </c>
       <c r="C62" s="50">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D62" s="67" t="s">
         <v>93</v>
       </c>
       <c r="E62" s="67" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="F62" s="69" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="G62" s="69" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="H62" s="69" t="s">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="I62" s="69" t="s">
-        <v>323</v>
+        <v>342</v>
       </c>
       <c r="J62" s="69" t="s">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="K62" s="70" t="s">
-        <v>390</v>
+        <v>441</v>
       </c>
       <c r="L62" s="55">
         <f>C62*K62</f>
-        <v>1.6800000000000002</v>
+        <v>7.54</v>
       </c>
     </row>
     <row r="63" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4760,35 +4844,35 @@
         <v>54</v>
       </c>
       <c r="C63" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D63" s="68" t="s">
         <v>94</v>
       </c>
       <c r="E63" s="68" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="F63" s="68" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="G63" s="68" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="H63" s="68" t="s">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="I63" s="68" t="s">
-        <v>323</v>
+        <v>342</v>
       </c>
       <c r="J63" s="68" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
       <c r="K63" s="71" t="s">
-        <v>416</v>
+        <v>442</v>
       </c>
       <c r="L63" s="57">
         <f t="shared" ref="L63" si="26">C63*K63</f>
-        <v>0.97</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="64" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4798,35 +4882,35 @@
         <v>55</v>
       </c>
       <c r="C64" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D64" s="67" t="s">
         <v>95</v>
       </c>
       <c r="E64" s="67" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="F64" s="69" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="G64" s="69" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="H64" s="69" t="s">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="I64" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J64" s="69" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="K64" s="70" t="s">
-        <v>417</v>
+        <v>443</v>
       </c>
       <c r="L64" s="55">
         <f>C64*K64</f>
-        <v>1.47</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="65" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4836,35 +4920,35 @@
         <v>56</v>
       </c>
       <c r="C65" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65" s="68" t="s">
         <v>96</v>
       </c>
       <c r="E65" s="68" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F65" s="68" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="G65" s="68" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="H65" s="68" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
       <c r="I65" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J65" s="68" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="K65" s="71" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="L65" s="57">
         <f t="shared" ref="L65" si="27">C65*K65</f>
-        <v>4</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="66" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4874,35 +4958,35 @@
         <v>57</v>
       </c>
       <c r="C66" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" s="67" t="s">
         <v>97</v>
       </c>
       <c r="E66" s="67" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F66" s="69" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="G66" s="69" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="H66" s="69" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="I66" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J66" s="69" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="K66" s="70" t="s">
-        <v>398</v>
+        <v>422</v>
       </c>
       <c r="L66" s="55">
         <f>C66*K66</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="67" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4912,35 +4996,35 @@
         <v>58</v>
       </c>
       <c r="C67" s="51">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D67" s="68" t="s">
         <v>98</v>
       </c>
       <c r="E67" s="68" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F67" s="68" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="G67" s="68" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="H67" s="68" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="I67" s="68" t="s">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c r="J67" s="68" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="K67" s="71" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="L67" s="57">
         <f t="shared" ref="L67" si="28">C67*K67</f>
-        <v>2.33</v>
+        <v>1.6800000000000002</v>
       </c>
     </row>
     <row r="68" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4956,29 +5040,29 @@
         <v>99</v>
       </c>
       <c r="E68" s="67" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F68" s="69" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="G68" s="69" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="H68" s="69" t="s">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="I68" s="69" t="s">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c r="J68" s="69" t="s">
-        <v>383</v>
+        <v>403</v>
       </c>
       <c r="K68" s="70" t="s">
-        <v>420</v>
+        <v>444</v>
       </c>
       <c r="L68" s="55">
         <f>C68*K68</f>
-        <v>0.39</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="69" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4988,35 +5072,35 @@
         <v>60</v>
       </c>
       <c r="C69" s="51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" s="68" t="s">
         <v>100</v>
       </c>
       <c r="E69" s="68" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F69" s="68" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="G69" s="68" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="H69" s="68" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="I69" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J69" s="68" t="s">
-        <v>384</v>
+        <v>404</v>
       </c>
       <c r="K69" s="71" t="s">
-        <v>421</v>
+        <v>445</v>
       </c>
       <c r="L69" s="57">
         <f t="shared" ref="L69" si="29">C69*K69</f>
-        <v>8.26</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="70" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -5026,35 +5110,35 @@
         <v>61</v>
       </c>
       <c r="C70" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D70" s="67" t="s">
         <v>101</v>
       </c>
       <c r="E70" s="67" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F70" s="69" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="G70" s="69" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="H70" s="69" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="I70" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J70" s="69" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="K70" s="70" t="s">
-        <v>422</v>
+        <v>446</v>
       </c>
       <c r="L70" s="55">
         <f>C70*K70</f>
-        <v>57.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5070,29 +5154,29 @@
         <v>102</v>
       </c>
       <c r="E71" s="68" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F71" s="68" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="G71" s="68" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="H71" s="68" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="I71" s="68" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J71" s="68" t="s">
-        <v>386</v>
+        <v>406</v>
       </c>
       <c r="K71" s="71" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="L71" s="57">
         <f t="shared" ref="L71" si="30">C71*K71</f>
-        <v>53.88</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="72" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -5102,134 +5186,324 @@
         <v>63</v>
       </c>
       <c r="C72" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D72" s="67" t="s">
         <v>103</v>
       </c>
       <c r="E72" s="67" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F72" s="69" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="G72" s="69" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="H72" s="69" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="I72" s="69" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J72" s="69" t="s">
-        <v>387</v>
+        <v>407</v>
       </c>
       <c r="K72" s="70" t="s">
-        <v>424</v>
+        <v>447</v>
       </c>
       <c r="L72" s="55">
         <f>C72*K72</f>
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="14"/>
+      <c r="B73" s="49">
+        <f>ROW(B73) - ROW($B$9)</f>
+        <v>64</v>
+      </c>
+      <c r="C73" s="51">
+        <v>1</v>
+      </c>
+      <c r="D73" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="E73" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="F73" s="68" t="s">
+        <v>240</v>
+      </c>
+      <c r="G73" s="68" t="s">
+        <v>270</v>
+      </c>
+      <c r="H73" s="68" t="s">
+        <v>336</v>
+      </c>
+      <c r="I73" s="68" t="s">
+        <v>342</v>
+      </c>
+      <c r="J73" s="68" t="s">
+        <v>408</v>
+      </c>
+      <c r="K73" s="71" t="s">
+        <v>448</v>
+      </c>
+      <c r="L73" s="57">
+        <f t="shared" ref="L73" si="31">C73*K73</f>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="14"/>
+      <c r="B74" s="48">
+        <f>ROW(B74) - ROW($B$9)</f>
+        <v>65</v>
+      </c>
+      <c r="C74" s="50">
+        <v>2</v>
+      </c>
+      <c r="D74" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="E74" s="67" t="s">
+        <v>172</v>
+      </c>
+      <c r="F74" s="69" t="s">
+        <v>241</v>
+      </c>
+      <c r="G74" s="69" t="s">
+        <v>269</v>
+      </c>
+      <c r="H74" s="69" t="s">
+        <v>337</v>
+      </c>
+      <c r="I74" s="69" t="s">
+        <v>342</v>
+      </c>
+      <c r="J74" s="69" t="s">
+        <v>409</v>
+      </c>
+      <c r="K74" s="70" t="s">
+        <v>449</v>
+      </c>
+      <c r="L74" s="55">
+        <f>C74*K74</f>
+        <v>8.26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="14"/>
+      <c r="B75" s="49">
+        <f>ROW(B75) - ROW($B$9)</f>
+        <v>66</v>
+      </c>
+      <c r="C75" s="51">
+        <v>1</v>
+      </c>
+      <c r="D75" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="E75" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="F75" s="68" t="s">
+        <v>242</v>
+      </c>
+      <c r="G75" s="68" t="s">
+        <v>271</v>
+      </c>
+      <c r="H75" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="I75" s="68" t="s">
+        <v>342</v>
+      </c>
+      <c r="J75" s="68" t="s">
+        <v>410</v>
+      </c>
+      <c r="K75" s="71" t="s">
+        <v>450</v>
+      </c>
+      <c r="L75" s="57">
+        <f t="shared" ref="L75" si="32">C75*K75</f>
+        <v>57.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="14"/>
+      <c r="B76" s="48">
+        <f>ROW(B76) - ROW($B$9)</f>
+        <v>67</v>
+      </c>
+      <c r="C76" s="50">
+        <v>2</v>
+      </c>
+      <c r="D76" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="E76" s="67" t="s">
+        <v>174</v>
+      </c>
+      <c r="F76" s="69" t="s">
+        <v>243</v>
+      </c>
+      <c r="G76" s="69" t="s">
+        <v>269</v>
+      </c>
+      <c r="H76" s="69" t="s">
+        <v>339</v>
+      </c>
+      <c r="I76" s="69" t="s">
+        <v>342</v>
+      </c>
+      <c r="J76" s="69" t="s">
+        <v>411</v>
+      </c>
+      <c r="K76" s="70" t="s">
+        <v>451</v>
+      </c>
+      <c r="L76" s="55">
+        <f>C76*K76</f>
+        <v>53.88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="14"/>
+      <c r="B77" s="49">
+        <f>ROW(B77) - ROW($B$9)</f>
+        <v>68</v>
+      </c>
+      <c r="C77" s="51">
+        <v>2</v>
+      </c>
+      <c r="D77" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="E77" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="F77" s="68" t="s">
+        <v>244</v>
+      </c>
+      <c r="G77" s="68" t="s">
+        <v>269</v>
+      </c>
+      <c r="H77" s="68" t="s">
+        <v>340</v>
+      </c>
+      <c r="I77" s="68" t="s">
+        <v>342</v>
+      </c>
+      <c r="J77" s="68" t="s">
+        <v>412</v>
+      </c>
+      <c r="K77" s="71" t="s">
+        <v>452</v>
+      </c>
+      <c r="L77" s="57">
+        <f t="shared" ref="L77" si="33">C77*K77</f>
         <v>1.32</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="58" t="s">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78" s="14"/>
+      <c r="B78" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C73" s="59"/>
-      <c r="D73" s="59"/>
-      <c r="E73" s="47"/>
-      <c r="F73" s="46"/>
-      <c r="G73" s="7" t="s">
+      <c r="C78" s="59"/>
+      <c r="D78" s="59"/>
+      <c r="E78" s="47"/>
+      <c r="F78" s="46"/>
+      <c r="G78" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J73" s="53" t="s">
+      <c r="J78" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="K73" s="54"/>
-      <c r="L73" s="56">
-        <f>SUM(L10:L72)</f>
-        <v>328.57999999999987</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="19"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A75" s="14"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="20"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
-      <c r="J76" s="9" t="s">
+      <c r="K78" s="54"/>
+      <c r="L78" s="56">
+        <f>SUM(L10:L77)</f>
+        <v>331.03999999999985</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79" s="14"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
+      <c r="K79" s="8"/>
+      <c r="L79" s="19"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80" s="14"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="20"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81" s="14"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="K76" s="9"/>
-      <c r="L76" s="20"/>
-    </row>
-    <row r="77" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
-      <c r="B77" s="44"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="16"/>
-      <c r="H77" s="16"/>
-      <c r="I77" s="16"/>
-      <c r="J77" s="16"/>
-      <c r="K77" s="16"/>
-      <c r="L77" s="21"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-    </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="20"/>
+    </row>
+    <row r="82" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="14"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="16"/>
+      <c r="L82" s="21"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B78:D78"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.46" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
@@ -5259,7 +5533,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>425</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5291,7 +5565,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>425</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -5307,7 +5581,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>426</v>
+        <v>454</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -5331,7 +5605,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="73" t="s">
-        <v>427</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -5339,7 +5613,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="74" t="s">
-        <v>428</v>
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -5347,7 +5621,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="73" t="s">
-        <v>428</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -5355,7 +5629,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="74" t="s">
-        <v>429</v>
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -5363,7 +5637,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="73" t="s">
-        <v>430</v>
+        <v>458</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -5371,7 +5645,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>431</v>
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -5379,7 +5653,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="73" t="s">
-        <v>432</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>